<commit_message>
i342--EIT2 suite file update for Jedi/d2/d1
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_04_jedi.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_04_jedi.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BBPw5sjxCCUVqKqDFh1VvlGl+6jBsyEv58ubpDIjFduKT4EttifNtZLgNn2j4jGi/bvDsFNRyO0+XWiClC3JHw==" workbookSaltValue="FQsz7bLsuDdqgfH6Nya7QA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240"/>
+    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,18 @@
     <definedName name="Z_179F0E1F_F6F7_410E_B883_54B8A90BA550_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
     <definedName name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
   </definedNames>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="122211" calcOnSave="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="392">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -867,15 +867,9 @@
     <t>suite_path = 04_Jedi_basic</t>
   </si>
   <si>
-    <t>PNMAIN_ENABLE_BITGEN=1</t>
-  </si>
-  <si>
     <t xml:space="preserve">cmd = python DEV/bin/run_radiant.py  --run-map-trce  --run-par-trce  </t>
   </si>
   <si>
-    <t>radiant=ng2_3</t>
-  </si>
-  <si>
     <t>=primitive</t>
   </si>
   <si>
@@ -909,9 +903,6 @@
     <t>00_primitive/00_common/09_FD1P3JX</t>
   </si>
   <si>
-    <t>00_primitive/00_common/10_FL1P3AZ</t>
-  </si>
-  <si>
     <t>00_primitive/00_common/11_IFD1P3BX</t>
   </si>
   <si>
@@ -1245,10 +1236,13 @@
     <t>sim</t>
   </si>
   <si>
-    <t>silicon_04_Jedi_v2.00</t>
-  </si>
-  <si>
     <t xml:space="preserve">cmd =  --check-conf=sim.conf,impl.conf --check-smart --sim-rtl   --synthesis=lse </t>
+  </si>
+  <si>
+    <t>silicon_04_Jedi_v2.01</t>
+  </si>
+  <si>
+    <t>radiant=ng3_0</t>
   </si>
 </sst>
 </file>
@@ -2551,64 +2545,31 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2620,7 +2581,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2640,17 +2607,44 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -5153,7 +5147,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7BDF45A0-A1B7-47D9-93C3-390BE88E3178}" diskRevisions="1" revisionId="1419" version="25">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F2C20D40-0E95-4DF4-B22D-E0617ADAE023}" diskRevisions="1" revisionId="1532" version="29">
   <header guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" dateTime="2020-10-15T13:42:26" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5354,6 +5348,38 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{F921E7B2-831E-4590-8E04-8405AAE4780A}" dateTime="2021-05-06T13:43:26" maxSheetId="5" userName="Jason Wang" r:id="rId26" minRId="1420" maxRId="1421">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6EFB87EC-1C45-4430-9A0D-8B70289C8E4E}" dateTime="2021-05-06T13:44:37" maxSheetId="5" userName="Jason Wang" r:id="rId27" minRId="1422" maxRId="1529">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{106EF222-343C-4FF5-9C0C-6CC5ED47CA9E}" dateTime="2021-05-06T13:45:23" maxSheetId="5" userName="Jason Wang" r:id="rId28" minRId="1531">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F2C20D40-0E95-4DF4-B22D-E0617ADAE023}" dateTime="2021-05-06T13:45:31" maxSheetId="5" userName="Jason Wang" r:id="rId29">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -11065,6 +11091,965 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1420" sId="1">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>silicon_04_Jedi_v2.00</t>
+      </is>
+    </oc>
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>silicon_04_Jedi_v2.01</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1421" sId="1">
+    <oc r="B6" t="inlineStr">
+      <is>
+        <t>PNMAIN_ENABLE_BITGEN=1</t>
+      </is>
+    </oc>
+    <nc r="B6"/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="1422" sId="2" ref="A10:XFD10" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A10:XFD10" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="30" formatCode="@"/>
+        <protection locked="0"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2" numFmtId="30">
+      <nc r="A10">
+        <v>8</v>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="E10" t="inlineStr">
+        <is>
+          <t>00_primitive/00_common/10_FL1P3AZ</t>
+        </is>
+      </nc>
+    </rcc>
+    <rfmt sheetId="2" sqref="L10" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="0" formatCode="General"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="S10" t="inlineStr">
+        <is>
+          <t>primitive</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="AD10" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rcc rId="1423" sId="2" numFmtId="30">
+    <oc r="A10">
+      <v>9</v>
+    </oc>
+    <nc r="A10">
+      <v>8</v>
+    </nc>
+  </rcc>
+  <rcc rId="1424" sId="2" numFmtId="30">
+    <oc r="A11">
+      <v>10</v>
+    </oc>
+    <nc r="A11">
+      <v>9</v>
+    </nc>
+  </rcc>
+  <rcc rId="1425" sId="2" numFmtId="30">
+    <oc r="A12">
+      <v>11</v>
+    </oc>
+    <nc r="A12">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcc rId="1426" sId="2" numFmtId="30">
+    <oc r="A13">
+      <v>12</v>
+    </oc>
+    <nc r="A13">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcc rId="1427" sId="2" numFmtId="30">
+    <oc r="A14">
+      <v>13</v>
+    </oc>
+    <nc r="A14">
+      <v>12</v>
+    </nc>
+  </rcc>
+  <rcc rId="1428" sId="2" numFmtId="30">
+    <oc r="A15">
+      <v>14</v>
+    </oc>
+    <nc r="A15">
+      <v>13</v>
+    </nc>
+  </rcc>
+  <rcc rId="1429" sId="2" numFmtId="30">
+    <oc r="A16">
+      <v>15</v>
+    </oc>
+    <nc r="A16">
+      <v>14</v>
+    </nc>
+  </rcc>
+  <rcc rId="1430" sId="2" numFmtId="30">
+    <oc r="A17">
+      <v>16</v>
+    </oc>
+    <nc r="A17">
+      <v>15</v>
+    </nc>
+  </rcc>
+  <rcc rId="1431" sId="2" numFmtId="30">
+    <oc r="A18">
+      <v>17</v>
+    </oc>
+    <nc r="A18">
+      <v>16</v>
+    </nc>
+  </rcc>
+  <rcc rId="1432" sId="2" numFmtId="30">
+    <oc r="A19">
+      <v>18</v>
+    </oc>
+    <nc r="A19">
+      <v>17</v>
+    </nc>
+  </rcc>
+  <rcc rId="1433" sId="2" numFmtId="30">
+    <oc r="A20">
+      <v>19</v>
+    </oc>
+    <nc r="A20">
+      <v>18</v>
+    </nc>
+  </rcc>
+  <rcc rId="1434" sId="2" numFmtId="30">
+    <oc r="A21">
+      <v>20</v>
+    </oc>
+    <nc r="A21">
+      <v>19</v>
+    </nc>
+  </rcc>
+  <rcc rId="1435" sId="2" numFmtId="30">
+    <oc r="A22">
+      <v>21</v>
+    </oc>
+    <nc r="A22">
+      <v>20</v>
+    </nc>
+  </rcc>
+  <rcc rId="1436" sId="2" numFmtId="30">
+    <oc r="A23">
+      <v>22</v>
+    </oc>
+    <nc r="A23">
+      <v>21</v>
+    </nc>
+  </rcc>
+  <rcc rId="1437" sId="2" numFmtId="30">
+    <oc r="A24">
+      <v>23</v>
+    </oc>
+    <nc r="A24">
+      <v>22</v>
+    </nc>
+  </rcc>
+  <rcc rId="1438" sId="2" numFmtId="30">
+    <oc r="A25">
+      <v>24</v>
+    </oc>
+    <nc r="A25">
+      <v>23</v>
+    </nc>
+  </rcc>
+  <rcc rId="1439" sId="2" numFmtId="30">
+    <oc r="A26">
+      <v>25</v>
+    </oc>
+    <nc r="A26">
+      <v>24</v>
+    </nc>
+  </rcc>
+  <rcc rId="1440" sId="2" numFmtId="30">
+    <oc r="A27">
+      <v>26</v>
+    </oc>
+    <nc r="A27">
+      <v>25</v>
+    </nc>
+  </rcc>
+  <rcc rId="1441" sId="2" numFmtId="30">
+    <oc r="A28">
+      <v>27</v>
+    </oc>
+    <nc r="A28">
+      <v>26</v>
+    </nc>
+  </rcc>
+  <rcc rId="1442" sId="2" numFmtId="30">
+    <oc r="A29">
+      <v>28</v>
+    </oc>
+    <nc r="A29">
+      <v>27</v>
+    </nc>
+  </rcc>
+  <rcc rId="1443" sId="2" numFmtId="30">
+    <oc r="A30">
+      <v>29</v>
+    </oc>
+    <nc r="A30">
+      <v>28</v>
+    </nc>
+  </rcc>
+  <rcc rId="1444" sId="2" numFmtId="30">
+    <oc r="A31">
+      <v>30</v>
+    </oc>
+    <nc r="A31">
+      <v>29</v>
+    </nc>
+  </rcc>
+  <rcc rId="1445" sId="2" numFmtId="30">
+    <oc r="A32">
+      <v>31</v>
+    </oc>
+    <nc r="A32">
+      <v>30</v>
+    </nc>
+  </rcc>
+  <rcc rId="1446" sId="2" numFmtId="30">
+    <oc r="A33">
+      <v>32</v>
+    </oc>
+    <nc r="A33">
+      <v>31</v>
+    </nc>
+  </rcc>
+  <rcc rId="1447" sId="2" numFmtId="30">
+    <oc r="A34">
+      <v>33</v>
+    </oc>
+    <nc r="A34">
+      <v>32</v>
+    </nc>
+  </rcc>
+  <rcc rId="1448" sId="2" numFmtId="30">
+    <oc r="A35">
+      <v>34</v>
+    </oc>
+    <nc r="A35">
+      <v>33</v>
+    </nc>
+  </rcc>
+  <rcc rId="1449" sId="2" numFmtId="30">
+    <oc r="A36">
+      <v>35</v>
+    </oc>
+    <nc r="A36">
+      <v>34</v>
+    </nc>
+  </rcc>
+  <rcc rId="1450" sId="2" numFmtId="30">
+    <oc r="A37">
+      <v>36</v>
+    </oc>
+    <nc r="A37">
+      <v>35</v>
+    </nc>
+  </rcc>
+  <rcc rId="1451" sId="2" numFmtId="30">
+    <oc r="A38">
+      <v>37</v>
+    </oc>
+    <nc r="A38">
+      <v>36</v>
+    </nc>
+  </rcc>
+  <rcc rId="1452" sId="2" numFmtId="30">
+    <oc r="A39">
+      <v>38</v>
+    </oc>
+    <nc r="A39">
+      <v>37</v>
+    </nc>
+  </rcc>
+  <rcc rId="1453" sId="2" numFmtId="30">
+    <oc r="A40">
+      <v>39</v>
+    </oc>
+    <nc r="A40">
+      <v>38</v>
+    </nc>
+  </rcc>
+  <rcc rId="1454" sId="2" numFmtId="30">
+    <oc r="A41">
+      <v>40</v>
+    </oc>
+    <nc r="A41">
+      <v>39</v>
+    </nc>
+  </rcc>
+  <rcc rId="1455" sId="2" numFmtId="30">
+    <oc r="A42">
+      <v>41</v>
+    </oc>
+    <nc r="A42">
+      <v>40</v>
+    </nc>
+  </rcc>
+  <rcc rId="1456" sId="2" numFmtId="30">
+    <oc r="A43">
+      <v>42</v>
+    </oc>
+    <nc r="A43">
+      <v>41</v>
+    </nc>
+  </rcc>
+  <rcc rId="1457" sId="2" numFmtId="30">
+    <oc r="A44">
+      <v>43</v>
+    </oc>
+    <nc r="A44">
+      <v>42</v>
+    </nc>
+  </rcc>
+  <rcc rId="1458" sId="2" numFmtId="30">
+    <oc r="A45">
+      <v>44</v>
+    </oc>
+    <nc r="A45">
+      <v>43</v>
+    </nc>
+  </rcc>
+  <rcc rId="1459" sId="2" numFmtId="30">
+    <oc r="A46">
+      <v>45</v>
+    </oc>
+    <nc r="A46">
+      <v>44</v>
+    </nc>
+  </rcc>
+  <rcc rId="1460" sId="2" numFmtId="30">
+    <oc r="A47">
+      <v>46</v>
+    </oc>
+    <nc r="A47">
+      <v>45</v>
+    </nc>
+  </rcc>
+  <rcc rId="1461" sId="2" numFmtId="30">
+    <oc r="A48">
+      <v>47</v>
+    </oc>
+    <nc r="A48">
+      <v>46</v>
+    </nc>
+  </rcc>
+  <rcc rId="1462" sId="2" numFmtId="30">
+    <oc r="A49">
+      <v>48</v>
+    </oc>
+    <nc r="A49">
+      <v>47</v>
+    </nc>
+  </rcc>
+  <rcc rId="1463" sId="2" numFmtId="30">
+    <oc r="A50">
+      <v>49</v>
+    </oc>
+    <nc r="A50">
+      <v>48</v>
+    </nc>
+  </rcc>
+  <rcc rId="1464" sId="2" numFmtId="30">
+    <oc r="A51">
+      <v>50</v>
+    </oc>
+    <nc r="A51">
+      <v>49</v>
+    </nc>
+  </rcc>
+  <rcc rId="1465" sId="2" numFmtId="30">
+    <oc r="A52">
+      <v>51</v>
+    </oc>
+    <nc r="A52">
+      <v>50</v>
+    </nc>
+  </rcc>
+  <rcc rId="1466" sId="2" numFmtId="30">
+    <oc r="A53">
+      <v>52</v>
+    </oc>
+    <nc r="A53">
+      <v>51</v>
+    </nc>
+  </rcc>
+  <rcc rId="1467" sId="2" numFmtId="30">
+    <oc r="A54">
+      <v>53</v>
+    </oc>
+    <nc r="A54">
+      <v>52</v>
+    </nc>
+  </rcc>
+  <rcc rId="1468" sId="2" numFmtId="30">
+    <oc r="A55">
+      <v>54</v>
+    </oc>
+    <nc r="A55">
+      <v>53</v>
+    </nc>
+  </rcc>
+  <rcc rId="1469" sId="2" numFmtId="30">
+    <oc r="A56">
+      <v>55</v>
+    </oc>
+    <nc r="A56">
+      <v>54</v>
+    </nc>
+  </rcc>
+  <rcc rId="1470" sId="2" numFmtId="30">
+    <oc r="A57">
+      <v>56</v>
+    </oc>
+    <nc r="A57">
+      <v>55</v>
+    </nc>
+  </rcc>
+  <rcc rId="1471" sId="2" numFmtId="30">
+    <oc r="A58">
+      <v>57</v>
+    </oc>
+    <nc r="A58">
+      <v>56</v>
+    </nc>
+  </rcc>
+  <rcc rId="1472" sId="2" numFmtId="30">
+    <oc r="A59">
+      <v>58</v>
+    </oc>
+    <nc r="A59">
+      <v>57</v>
+    </nc>
+  </rcc>
+  <rcc rId="1473" sId="2" numFmtId="30">
+    <oc r="A60">
+      <v>59</v>
+    </oc>
+    <nc r="A60">
+      <v>58</v>
+    </nc>
+  </rcc>
+  <rcc rId="1474" sId="2" numFmtId="30">
+    <oc r="A61">
+      <v>60</v>
+    </oc>
+    <nc r="A61">
+      <v>59</v>
+    </nc>
+  </rcc>
+  <rcc rId="1475" sId="2" numFmtId="30">
+    <oc r="A62">
+      <v>61</v>
+    </oc>
+    <nc r="A62">
+      <v>60</v>
+    </nc>
+  </rcc>
+  <rcc rId="1476" sId="2" numFmtId="30">
+    <oc r="A63">
+      <v>62</v>
+    </oc>
+    <nc r="A63">
+      <v>61</v>
+    </nc>
+  </rcc>
+  <rcc rId="1477" sId="2" numFmtId="30">
+    <oc r="A64">
+      <v>63</v>
+    </oc>
+    <nc r="A64">
+      <v>62</v>
+    </nc>
+  </rcc>
+  <rcc rId="1478" sId="2" numFmtId="30">
+    <oc r="A65">
+      <v>64</v>
+    </oc>
+    <nc r="A65">
+      <v>63</v>
+    </nc>
+  </rcc>
+  <rcc rId="1479" sId="2" numFmtId="30">
+    <oc r="A66">
+      <v>65</v>
+    </oc>
+    <nc r="A66">
+      <v>64</v>
+    </nc>
+  </rcc>
+  <rcc rId="1480" sId="2" numFmtId="30">
+    <oc r="A67">
+      <v>66</v>
+    </oc>
+    <nc r="A67">
+      <v>65</v>
+    </nc>
+  </rcc>
+  <rcc rId="1481" sId="2" numFmtId="30">
+    <oc r="A68">
+      <v>67</v>
+    </oc>
+    <nc r="A68">
+      <v>66</v>
+    </nc>
+  </rcc>
+  <rcc rId="1482" sId="2" numFmtId="30">
+    <oc r="A69">
+      <v>68</v>
+    </oc>
+    <nc r="A69">
+      <v>67</v>
+    </nc>
+  </rcc>
+  <rcc rId="1483" sId="2" numFmtId="30">
+    <oc r="A70">
+      <v>69</v>
+    </oc>
+    <nc r="A70">
+      <v>68</v>
+    </nc>
+  </rcc>
+  <rcc rId="1484" sId="2" numFmtId="30">
+    <oc r="A71">
+      <v>70</v>
+    </oc>
+    <nc r="A71">
+      <v>69</v>
+    </nc>
+  </rcc>
+  <rcc rId="1485" sId="2" numFmtId="30">
+    <oc r="A72">
+      <v>71</v>
+    </oc>
+    <nc r="A72">
+      <v>70</v>
+    </nc>
+  </rcc>
+  <rcc rId="1486" sId="2" numFmtId="30">
+    <oc r="A73">
+      <v>72</v>
+    </oc>
+    <nc r="A73">
+      <v>71</v>
+    </nc>
+  </rcc>
+  <rcc rId="1487" sId="2" numFmtId="30">
+    <oc r="A74">
+      <v>73</v>
+    </oc>
+    <nc r="A74">
+      <v>72</v>
+    </nc>
+  </rcc>
+  <rcc rId="1488" sId="2" numFmtId="30">
+    <oc r="A75">
+      <v>74</v>
+    </oc>
+    <nc r="A75">
+      <v>73</v>
+    </nc>
+  </rcc>
+  <rcc rId="1489" sId="2" numFmtId="30">
+    <oc r="A76">
+      <v>75</v>
+    </oc>
+    <nc r="A76">
+      <v>74</v>
+    </nc>
+  </rcc>
+  <rcc rId="1490" sId="2" numFmtId="30">
+    <oc r="A77">
+      <v>76</v>
+    </oc>
+    <nc r="A77">
+      <v>75</v>
+    </nc>
+  </rcc>
+  <rcc rId="1491" sId="2" numFmtId="30">
+    <oc r="A78">
+      <v>77</v>
+    </oc>
+    <nc r="A78">
+      <v>76</v>
+    </nc>
+  </rcc>
+  <rcc rId="1492" sId="2" numFmtId="30">
+    <oc r="A79">
+      <v>78</v>
+    </oc>
+    <nc r="A79">
+      <v>77</v>
+    </nc>
+  </rcc>
+  <rcc rId="1493" sId="2" numFmtId="30">
+    <oc r="A80">
+      <v>79</v>
+    </oc>
+    <nc r="A80">
+      <v>78</v>
+    </nc>
+  </rcc>
+  <rcc rId="1494" sId="2" numFmtId="30">
+    <oc r="A81">
+      <v>80</v>
+    </oc>
+    <nc r="A81">
+      <v>79</v>
+    </nc>
+  </rcc>
+  <rcc rId="1495" sId="2" numFmtId="30">
+    <oc r="A82">
+      <v>81</v>
+    </oc>
+    <nc r="A82">
+      <v>80</v>
+    </nc>
+  </rcc>
+  <rcc rId="1496" sId="2" numFmtId="30">
+    <oc r="A83">
+      <v>82</v>
+    </oc>
+    <nc r="A83">
+      <v>81</v>
+    </nc>
+  </rcc>
+  <rcc rId="1497" sId="2" numFmtId="30">
+    <oc r="A84">
+      <v>83</v>
+    </oc>
+    <nc r="A84">
+      <v>82</v>
+    </nc>
+  </rcc>
+  <rcc rId="1498" sId="2" numFmtId="30">
+    <oc r="A85">
+      <v>84</v>
+    </oc>
+    <nc r="A85">
+      <v>83</v>
+    </nc>
+  </rcc>
+  <rcc rId="1499" sId="2" numFmtId="30">
+    <oc r="A86">
+      <v>85</v>
+    </oc>
+    <nc r="A86">
+      <v>84</v>
+    </nc>
+  </rcc>
+  <rcc rId="1500" sId="2" numFmtId="30">
+    <oc r="A87">
+      <v>86</v>
+    </oc>
+    <nc r="A87">
+      <v>85</v>
+    </nc>
+  </rcc>
+  <rcc rId="1501" sId="2" numFmtId="30">
+    <oc r="A88">
+      <v>87</v>
+    </oc>
+    <nc r="A88">
+      <v>86</v>
+    </nc>
+  </rcc>
+  <rcc rId="1502" sId="2" numFmtId="30">
+    <oc r="A89">
+      <v>88</v>
+    </oc>
+    <nc r="A89">
+      <v>87</v>
+    </nc>
+  </rcc>
+  <rcc rId="1503" sId="2" numFmtId="30">
+    <oc r="A90">
+      <v>89</v>
+    </oc>
+    <nc r="A90">
+      <v>88</v>
+    </nc>
+  </rcc>
+  <rcc rId="1504" sId="2" numFmtId="30">
+    <oc r="A91">
+      <v>90</v>
+    </oc>
+    <nc r="A91">
+      <v>89</v>
+    </nc>
+  </rcc>
+  <rcc rId="1505" sId="2" numFmtId="30">
+    <oc r="A92">
+      <v>91</v>
+    </oc>
+    <nc r="A92">
+      <v>90</v>
+    </nc>
+  </rcc>
+  <rcc rId="1506" sId="2" numFmtId="30">
+    <oc r="A93">
+      <v>92</v>
+    </oc>
+    <nc r="A93">
+      <v>91</v>
+    </nc>
+  </rcc>
+  <rcc rId="1507" sId="2" numFmtId="30">
+    <oc r="A94">
+      <v>93</v>
+    </oc>
+    <nc r="A94">
+      <v>92</v>
+    </nc>
+  </rcc>
+  <rcc rId="1508" sId="2" numFmtId="30">
+    <oc r="A95">
+      <v>94</v>
+    </oc>
+    <nc r="A95">
+      <v>93</v>
+    </nc>
+  </rcc>
+  <rcc rId="1509" sId="2" numFmtId="30">
+    <oc r="A96">
+      <v>95</v>
+    </oc>
+    <nc r="A96">
+      <v>94</v>
+    </nc>
+  </rcc>
+  <rcc rId="1510" sId="2" numFmtId="30">
+    <oc r="A97">
+      <v>96</v>
+    </oc>
+    <nc r="A97">
+      <v>95</v>
+    </nc>
+  </rcc>
+  <rcc rId="1511" sId="2" numFmtId="30">
+    <oc r="A98">
+      <v>97</v>
+    </oc>
+    <nc r="A98">
+      <v>96</v>
+    </nc>
+  </rcc>
+  <rcc rId="1512" sId="2" numFmtId="30">
+    <oc r="A99">
+      <v>98</v>
+    </oc>
+    <nc r="A99">
+      <v>97</v>
+    </nc>
+  </rcc>
+  <rcc rId="1513" sId="2" numFmtId="30">
+    <oc r="A100">
+      <v>99</v>
+    </oc>
+    <nc r="A100">
+      <v>98</v>
+    </nc>
+  </rcc>
+  <rcc rId="1514" sId="2" numFmtId="30">
+    <oc r="A101">
+      <v>100</v>
+    </oc>
+    <nc r="A101">
+      <v>99</v>
+    </nc>
+  </rcc>
+  <rcc rId="1515" sId="2" numFmtId="30">
+    <oc r="A102">
+      <v>101</v>
+    </oc>
+    <nc r="A102">
+      <v>100</v>
+    </nc>
+  </rcc>
+  <rcc rId="1516" sId="2" numFmtId="30">
+    <oc r="A103">
+      <v>102</v>
+    </oc>
+    <nc r="A103">
+      <v>101</v>
+    </nc>
+  </rcc>
+  <rcc rId="1517" sId="2" numFmtId="30">
+    <oc r="A104">
+      <v>103</v>
+    </oc>
+    <nc r="A104">
+      <v>102</v>
+    </nc>
+  </rcc>
+  <rcc rId="1518" sId="2" numFmtId="30">
+    <oc r="A105">
+      <v>104</v>
+    </oc>
+    <nc r="A105">
+      <v>103</v>
+    </nc>
+  </rcc>
+  <rcc rId="1519" sId="2" numFmtId="30">
+    <oc r="A106">
+      <v>105</v>
+    </oc>
+    <nc r="A106">
+      <v>104</v>
+    </nc>
+  </rcc>
+  <rcc rId="1520" sId="2" numFmtId="30">
+    <oc r="A107">
+      <v>106</v>
+    </oc>
+    <nc r="A107">
+      <v>105</v>
+    </nc>
+  </rcc>
+  <rcc rId="1521" sId="2" numFmtId="30">
+    <oc r="A108">
+      <v>107</v>
+    </oc>
+    <nc r="A108">
+      <v>106</v>
+    </nc>
+  </rcc>
+  <rcc rId="1522" sId="2" numFmtId="30">
+    <oc r="A109">
+      <v>108</v>
+    </oc>
+    <nc r="A109">
+      <v>107</v>
+    </nc>
+  </rcc>
+  <rcc rId="1523" sId="2" numFmtId="30">
+    <oc r="A110">
+      <v>109</v>
+    </oc>
+    <nc r="A110">
+      <v>108</v>
+    </nc>
+  </rcc>
+  <rcc rId="1524" sId="2" numFmtId="30">
+    <oc r="A111">
+      <v>110</v>
+    </oc>
+    <nc r="A111">
+      <v>109</v>
+    </nc>
+  </rcc>
+  <rcc rId="1525" sId="2" numFmtId="30">
+    <oc r="A112">
+      <v>111</v>
+    </oc>
+    <nc r="A112">
+      <v>110</v>
+    </nc>
+  </rcc>
+  <rcc rId="1526" sId="2" numFmtId="30">
+    <oc r="A113">
+      <v>112</v>
+    </oc>
+    <nc r="A113">
+      <v>111</v>
+    </nc>
+  </rcc>
+  <rcc rId="1527" sId="2" numFmtId="30">
+    <oc r="A114">
+      <v>113</v>
+    </oc>
+    <nc r="A114">
+      <v>112</v>
+    </nc>
+  </rcc>
+  <rcc rId="1528" sId="2" numFmtId="30">
+    <oc r="A115">
+      <v>114</v>
+    </oc>
+    <nc r="A115">
+      <v>113</v>
+    </nc>
+  </rcc>
+  <rcc rId="1529" sId="2" numFmtId="30">
+    <oc r="A116">
+      <v>115</v>
+    </oc>
+    <nc r="A116">
+      <v>114</v>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog28.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1531" sId="1">
+    <oc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng2_3</t>
+      </is>
+    </oc>
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>radiant=ng3_0</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
 </revisions>
 </file>
 
@@ -19486,7 +20471,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
   <userInfo guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" name="Cherry (Ying) Xu" id="-707422276" dateTime="2020-11-23T15:52:35"/>
 </users>
@@ -19781,8 +20766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -19813,7 +20798,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -19833,16 +20818,13 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>266</v>
-      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -19850,7 +20832,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>268</v>
+        <v>391</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -19887,7 +20869,7 @@
         <v>108</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -19898,7 +20880,7 @@
         <v>87</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -19909,7 +20891,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -19936,7 +20918,7 @@
         <v>108</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -19947,7 +20929,7 @@
         <v>87</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -19958,7 +20940,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -19970,12 +20952,12 @@
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B27" sqref="B27"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}">
-      <selection activeCell="C37" sqref="C37"/>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -19984,8 +20966,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
+    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}">
+      <selection activeCell="C37" sqref="C37"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -19998,14 +20980,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD117"/>
+  <dimension ref="A1:AD116"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -20170,13 +21152,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -20184,13 +21166,13 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -20198,10 +21180,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD5" s="2" t="s">
         <v>261</v>
@@ -20212,13 +21194,13 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -20226,13 +21208,13 @@
         <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -20240,13 +21222,13 @@
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -20254,13 +21236,13 @@
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -20268,13 +21250,13 @@
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -20282,13 +21264,13 @@
         <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -20296,13 +21278,13 @@
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -20310,13 +21292,13 @@
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:30">
@@ -20324,13 +21306,13 @@
         <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15" spans="1:30">
@@ -20338,13 +21320,13 @@
         <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -20352,13 +21334,13 @@
         <v>14</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD16" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:30">
@@ -20366,13 +21348,13 @@
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="18" spans="1:30">
@@ -20380,13 +21362,13 @@
         <v>16</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD18" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="19" spans="1:30">
@@ -20394,13 +21376,13 @@
         <v>17</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="20" spans="1:30">
@@ -20408,13 +21390,13 @@
         <v>18</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD20" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="21" spans="1:30">
@@ -20422,13 +21404,13 @@
         <v>19</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="22" spans="1:30">
@@ -20436,13 +21418,13 @@
         <v>20</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD22" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:30">
@@ -20450,13 +21432,13 @@
         <v>21</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD23" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="24" spans="1:30">
@@ -20464,13 +21446,13 @@
         <v>22</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD24" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:30">
@@ -20478,10 +21460,10 @@
         <v>23</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD25" s="2" t="s">
         <v>261</v>
@@ -20492,10 +21474,10 @@
         <v>24</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD26" s="2" t="s">
         <v>261</v>
@@ -20506,10 +21488,10 @@
         <v>25</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD27" s="2" t="s">
         <v>261</v>
@@ -20520,10 +21502,10 @@
         <v>26</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD28" s="2" t="s">
         <v>261</v>
@@ -20534,13 +21516,13 @@
         <v>27</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD29" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="30" spans="1:30">
@@ -20548,13 +21530,13 @@
         <v>28</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD30" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31" spans="1:30">
@@ -20562,13 +21544,13 @@
         <v>29</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD31" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="32" spans="1:30">
@@ -20576,13 +21558,13 @@
         <v>30</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD32" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="33" spans="1:30">
@@ -20590,13 +21572,16 @@
         <v>31</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>302</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD33" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="34" spans="1:30">
@@ -20604,16 +21589,16 @@
         <v>32</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD34" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:30">
@@ -20621,16 +21606,13 @@
         <v>33</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="O35" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD35" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="36" spans="1:30">
@@ -20638,13 +21620,13 @@
         <v>34</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD36" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="37" spans="1:30">
@@ -20652,13 +21634,13 @@
         <v>35</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD37" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:30">
@@ -20666,13 +21648,13 @@
         <v>36</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD38" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="39" spans="1:30">
@@ -20680,13 +21662,13 @@
         <v>37</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD39" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:30">
@@ -20694,13 +21676,13 @@
         <v>38</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD40" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="41" spans="1:30">
@@ -20708,13 +21690,13 @@
         <v>39</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD41" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="42" spans="1:30">
@@ -20722,13 +21704,13 @@
         <v>40</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD42" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="43" spans="1:30">
@@ -20736,13 +21718,13 @@
         <v>41</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD43" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="44" spans="1:30">
@@ -20750,13 +21732,13 @@
         <v>42</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD44" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="45" spans="1:30">
@@ -20764,13 +21746,13 @@
         <v>43</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD45" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="46" spans="1:30">
@@ -20778,13 +21760,13 @@
         <v>44</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD46" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="47" spans="1:30">
@@ -20792,13 +21774,13 @@
         <v>45</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD47" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="48" spans="1:30">
@@ -20806,13 +21788,13 @@
         <v>46</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD48" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="49" spans="1:30">
@@ -20820,13 +21802,13 @@
         <v>47</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD49" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="50" spans="1:30">
@@ -20834,13 +21816,13 @@
         <v>48</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD50" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="51" spans="1:30">
@@ -20848,13 +21830,13 @@
         <v>49</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD51" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="52" spans="1:30">
@@ -20862,13 +21844,13 @@
         <v>50</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="S52" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD52" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="53" spans="1:30">
@@ -20876,13 +21858,13 @@
         <v>51</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="S53" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD53" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="54" spans="1:30">
@@ -20890,13 +21872,13 @@
         <v>52</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="S54" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD54" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="55" spans="1:30">
@@ -20904,13 +21886,13 @@
         <v>53</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="S55" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD55" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="56" spans="1:30">
@@ -20918,13 +21900,13 @@
         <v>54</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="S56" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD56" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="57" spans="1:30">
@@ -20932,13 +21914,13 @@
         <v>55</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="S57" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD57" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="58" spans="1:30">
@@ -20946,13 +21928,13 @@
         <v>56</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="S58" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD58" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="59" spans="1:30">
@@ -20960,13 +21942,13 @@
         <v>57</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="S59" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD59" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="60" spans="1:30">
@@ -20974,13 +21956,13 @@
         <v>58</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="S60" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD60" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="61" spans="1:30">
@@ -20988,13 +21970,13 @@
         <v>59</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="S61" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD61" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="62" spans="1:30">
@@ -21002,13 +21984,13 @@
         <v>60</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="S62" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD62" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="63" spans="1:30">
@@ -21016,13 +21998,13 @@
         <v>61</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="S63" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD63" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="64" spans="1:30">
@@ -21030,13 +22012,13 @@
         <v>62</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="S64" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD64" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="65" spans="1:30">
@@ -21044,13 +22026,13 @@
         <v>63</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="S65" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD65" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="66" spans="1:30">
@@ -21058,13 +22040,13 @@
         <v>64</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="S66" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD66" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="67" spans="1:30">
@@ -21072,13 +22054,13 @@
         <v>65</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="S67" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD67" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="68" spans="1:30">
@@ -21086,13 +22068,13 @@
         <v>66</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="S68" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD68" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="69" spans="1:30">
@@ -21100,13 +22082,13 @@
         <v>67</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="S69" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD69" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="70" spans="1:30">
@@ -21114,13 +22096,13 @@
         <v>68</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="S70" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD70" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="71" spans="1:30">
@@ -21128,13 +22110,13 @@
         <v>69</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="S71" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD71" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="72" spans="1:30">
@@ -21142,13 +22124,13 @@
         <v>70</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="S72" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD72" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="73" spans="1:30">
@@ -21156,13 +22138,13 @@
         <v>71</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="S73" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD73" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="74" spans="1:30">
@@ -21170,13 +22152,13 @@
         <v>72</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="S74" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD74" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="75" spans="1:30">
@@ -21184,13 +22166,13 @@
         <v>73</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="S75" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD75" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="76" spans="1:30">
@@ -21198,13 +22180,13 @@
         <v>74</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="S76" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD76" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="77" spans="1:30">
@@ -21212,13 +22194,13 @@
         <v>75</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="S77" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD77" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="78" spans="1:30">
@@ -21226,13 +22208,13 @@
         <v>76</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="S78" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD78" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="79" spans="1:30">
@@ -21240,13 +22222,13 @@
         <v>77</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="S79" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD79" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="80" spans="1:30">
@@ -21254,13 +22236,13 @@
         <v>78</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="S80" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD80" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="81" spans="1:30">
@@ -21268,13 +22250,13 @@
         <v>79</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="S81" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD81" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="82" spans="1:30">
@@ -21282,13 +22264,13 @@
         <v>80</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="S82" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD82" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="83" spans="1:30">
@@ -21296,13 +22278,13 @@
         <v>81</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="S83" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD83" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="84" spans="1:30">
@@ -21310,13 +22292,13 @@
         <v>82</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="S84" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD84" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="85" spans="1:30">
@@ -21324,13 +22306,13 @@
         <v>83</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="S85" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD85" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="86" spans="1:30">
@@ -21338,13 +22320,13 @@
         <v>84</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="S86" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD86" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="87" spans="1:30">
@@ -21352,13 +22334,13 @@
         <v>85</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="S87" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD87" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="88" spans="1:30">
@@ -21366,13 +22348,13 @@
         <v>86</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="S88" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD88" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="89" spans="1:30">
@@ -21380,13 +22362,13 @@
         <v>87</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="S89" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD89" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="90" spans="1:30">
@@ -21394,13 +22376,13 @@
         <v>88</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="S90" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD90" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="91" spans="1:30">
@@ -21408,13 +22390,13 @@
         <v>89</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="S91" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD91" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="92" spans="1:30">
@@ -21422,13 +22404,13 @@
         <v>90</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="S92" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD92" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="93" spans="1:30">
@@ -21436,13 +22418,13 @@
         <v>91</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="S93" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD93" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="94" spans="1:30">
@@ -21450,13 +22432,13 @@
         <v>92</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="S94" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD94" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="95" spans="1:30">
@@ -21464,13 +22446,13 @@
         <v>93</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="S95" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD95" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="96" spans="1:30">
@@ -21478,13 +22460,13 @@
         <v>94</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="S96" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD96" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="97" spans="1:30">
@@ -21492,13 +22474,13 @@
         <v>95</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="S97" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD97" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="98" spans="1:30">
@@ -21506,13 +22488,13 @@
         <v>96</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="S98" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD98" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="99" spans="1:30">
@@ -21520,13 +22502,16 @@
         <v>97</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
+      </c>
+      <c r="O99" s="2" t="s">
+        <v>369</v>
       </c>
       <c r="S99" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD99" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="100" spans="1:30">
@@ -21534,16 +22519,13 @@
         <v>98</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="O100" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="S100" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD100" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="101" spans="1:30">
@@ -21551,13 +22533,13 @@
         <v>99</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="S101" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD101" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="102" spans="1:30">
@@ -21565,13 +22547,13 @@
         <v>100</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="S102" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD102" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="103" spans="1:30">
@@ -21579,13 +22561,13 @@
         <v>101</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="S103" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD103" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="104" spans="1:30">
@@ -21593,13 +22575,13 @@
         <v>102</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="S104" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD104" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="105" spans="1:30">
@@ -21607,13 +22589,13 @@
         <v>103</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="S105" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD105" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="106" spans="1:30">
@@ -21621,13 +22603,13 @@
         <v>104</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="S106" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD106" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="107" spans="1:30">
@@ -21635,13 +22617,13 @@
         <v>105</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="S107" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD107" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="108" spans="1:30">
@@ -21649,13 +22631,13 @@
         <v>106</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="S108" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD108" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="109" spans="1:30">
@@ -21663,13 +22645,13 @@
         <v>107</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="S109" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD109" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="110" spans="1:30">
@@ -21677,13 +22659,13 @@
         <v>108</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="S110" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD110" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="111" spans="1:30">
@@ -21691,10 +22673,10 @@
         <v>109</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="S111" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD111" s="2" t="s">
         <v>261</v>
@@ -21705,13 +22687,13 @@
         <v>110</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="S112" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD112" s="2" t="s">
-        <v>261</v>
+        <v>388</v>
       </c>
     </row>
     <row r="113" spans="1:30">
@@ -21719,13 +22701,13 @@
         <v>111</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="S113" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD113" s="2" t="s">
-        <v>391</v>
+        <v>261</v>
       </c>
     </row>
     <row r="114" spans="1:30">
@@ -21733,10 +22715,10 @@
         <v>112</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="S114" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD114" s="2" t="s">
         <v>261</v>
@@ -21747,10 +22729,10 @@
         <v>113</v>
       </c>
       <c r="E115" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="S115" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="S115" s="2" t="s">
-        <v>390</v>
       </c>
       <c r="AD115" s="2" t="s">
         <v>261</v>
@@ -21761,26 +22743,12 @@
         <v>114</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="S116" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AD116" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="117" spans="1:30">
-      <c r="A117" s="2">
-        <v>115</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="S117" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="AD117" s="2" t="s">
         <v>261</v>
       </c>
     </row>
@@ -21790,17 +22758,17 @@
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="B116" sqref="B116"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A2:AD2"/>
     </customSheetView>
-    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" scale="70" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="F87" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="O114" sqref="O114"/>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A2:AD2"/>
+      <autoFilter ref="A2:Y2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -21809,12 +22777,12 @@
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" scale="70" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="F87" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="O114" sqref="O114"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:AD2"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -21950,17 +22918,17 @@
       <c r="E111" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F111" s="104" t="s">
+      <c r="F111" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="G111" s="105"/>
-      <c r="H111" s="105"/>
-      <c r="I111" s="105"/>
-      <c r="J111" s="105"/>
-      <c r="K111" s="105"/>
-      <c r="L111" s="105"/>
-      <c r="M111" s="105"/>
-      <c r="N111" s="106"/>
+      <c r="G111" s="74"/>
+      <c r="H111" s="74"/>
+      <c r="I111" s="74"/>
+      <c r="J111" s="74"/>
+      <c r="K111" s="74"/>
+      <c r="L111" s="74"/>
+      <c r="M111" s="74"/>
+      <c r="N111" s="75"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -22824,7 +23792,7 @@
       <c r="A147" s="26">
         <v>1</v>
       </c>
-      <c r="B147" s="89" t="s">
+      <c r="B147" s="76" t="s">
         <v>3</v>
       </c>
       <c r="C147" s="27" t="s">
@@ -22850,7 +23818,7 @@
       <c r="A148" s="26">
         <v>2</v>
       </c>
-      <c r="B148" s="90"/>
+      <c r="B148" s="77"/>
       <c r="C148" s="28" t="s">
         <v>130</v>
       </c>
@@ -22872,7 +23840,7 @@
       <c r="A149" s="26">
         <v>3</v>
       </c>
-      <c r="B149" s="90"/>
+      <c r="B149" s="77"/>
       <c r="C149" s="28" t="s">
         <v>9</v>
       </c>
@@ -22892,7 +23860,7 @@
       <c r="A150" s="26">
         <v>4</v>
       </c>
-      <c r="B150" s="90"/>
+      <c r="B150" s="77"/>
       <c r="C150" s="28" t="s">
         <v>132</v>
       </c>
@@ -22916,7 +23884,7 @@
       <c r="A151" s="26">
         <v>5</v>
       </c>
-      <c r="B151" s="90"/>
+      <c r="B151" s="77"/>
       <c r="C151" s="27" t="s">
         <v>134</v>
       </c>
@@ -22940,7 +23908,7 @@
       <c r="A152" s="26">
         <v>6</v>
       </c>
-      <c r="B152" s="90"/>
+      <c r="B152" s="77"/>
       <c r="C152" s="27" t="s">
         <v>138</v>
       </c>
@@ -22964,7 +23932,7 @@
       <c r="A153" s="26">
         <v>7</v>
       </c>
-      <c r="B153" s="90"/>
+      <c r="B153" s="77"/>
       <c r="C153" s="28" t="s">
         <v>141</v>
       </c>
@@ -22986,7 +23954,7 @@
       <c r="A154" s="26">
         <v>8</v>
       </c>
-      <c r="B154" s="90"/>
+      <c r="B154" s="77"/>
       <c r="C154" s="27" t="s">
         <v>142</v>
       </c>
@@ -23010,7 +23978,7 @@
       <c r="A155" s="26">
         <v>9</v>
       </c>
-      <c r="B155" s="90"/>
+      <c r="B155" s="77"/>
       <c r="C155" s="27" t="s">
         <v>143</v>
       </c>
@@ -23034,7 +24002,7 @@
       <c r="A156" s="26">
         <v>10</v>
       </c>
-      <c r="B156" s="90"/>
+      <c r="B156" s="77"/>
       <c r="C156" s="28" t="s">
         <v>144</v>
       </c>
@@ -23058,7 +24026,7 @@
       <c r="A157" s="26">
         <v>11</v>
       </c>
-      <c r="B157" s="90"/>
+      <c r="B157" s="77"/>
       <c r="C157" s="28" t="s">
         <v>145</v>
       </c>
@@ -23082,7 +24050,7 @@
       <c r="A158" s="26">
         <v>12</v>
       </c>
-      <c r="B158" s="90"/>
+      <c r="B158" s="77"/>
       <c r="C158" s="28" t="s">
         <v>147</v>
       </c>
@@ -23104,7 +24072,7 @@
       <c r="A159" s="26">
         <v>13</v>
       </c>
-      <c r="B159" s="84"/>
+      <c r="B159" s="78"/>
       <c r="C159" s="28" t="s">
         <v>55</v>
       </c>
@@ -23128,7 +24096,7 @@
       <c r="A160" s="26">
         <v>14</v>
       </c>
-      <c r="B160" s="80" t="s">
+      <c r="B160" s="71" t="s">
         <v>4</v>
       </c>
       <c r="C160" s="28" t="s">
@@ -23154,7 +24122,7 @@
       <c r="A161" s="26">
         <v>15</v>
       </c>
-      <c r="B161" s="79"/>
+      <c r="B161" s="72"/>
       <c r="C161" s="28" t="s">
         <v>155</v>
       </c>
@@ -23178,7 +24146,7 @@
       <c r="A162" s="26">
         <v>16</v>
       </c>
-      <c r="B162" s="89" t="s">
+      <c r="B162" s="76" t="s">
         <v>5</v>
       </c>
       <c r="C162" s="28" t="s">
@@ -23202,7 +24170,7 @@
       <c r="A163" s="26">
         <v>17</v>
       </c>
-      <c r="B163" s="107"/>
+      <c r="B163" s="79"/>
       <c r="C163" s="27" t="s">
         <v>159</v>
       </c>
@@ -23224,7 +24192,7 @@
       <c r="A164" s="26">
         <v>18</v>
       </c>
-      <c r="B164" s="84"/>
+      <c r="B164" s="78"/>
       <c r="C164" s="27" t="s">
         <v>161</v>
       </c>
@@ -23244,7 +24212,7 @@
       <c r="A165" s="26">
         <v>19</v>
       </c>
-      <c r="B165" s="80" t="s">
+      <c r="B165" s="71" t="s">
         <v>6</v>
       </c>
       <c r="C165" s="28" t="s">
@@ -23268,7 +24236,7 @@
       <c r="A166" s="26">
         <v>20</v>
       </c>
-      <c r="B166" s="79"/>
+      <c r="B166" s="72"/>
       <c r="C166" s="28" t="s">
         <v>166</v>
       </c>
@@ -23288,7 +24256,7 @@
       <c r="A167" s="26">
         <v>21</v>
       </c>
-      <c r="B167" s="79"/>
+      <c r="B167" s="72"/>
       <c r="C167" s="28" t="s">
         <v>167</v>
       </c>
@@ -23308,7 +24276,7 @@
       <c r="A168" s="26">
         <v>22</v>
       </c>
-      <c r="B168" s="79"/>
+      <c r="B168" s="72"/>
       <c r="C168" s="28" t="s">
         <v>168</v>
       </c>
@@ -23328,7 +24296,7 @@
       <c r="A169" s="26">
         <v>23</v>
       </c>
-      <c r="B169" s="79"/>
+      <c r="B169" s="72"/>
       <c r="C169" s="28" t="s">
         <v>169</v>
       </c>
@@ -23348,7 +24316,7 @@
       <c r="A170" s="26">
         <v>24</v>
       </c>
-      <c r="B170" s="79"/>
+      <c r="B170" s="72"/>
       <c r="C170" s="28" t="s">
         <v>170</v>
       </c>
@@ -23368,7 +24336,7 @@
       <c r="A171" s="26">
         <v>25</v>
       </c>
-      <c r="B171" s="79"/>
+      <c r="B171" s="72"/>
       <c r="C171" s="28" t="s">
         <v>171</v>
       </c>
@@ -23388,7 +24356,7 @@
       <c r="A172" s="26">
         <v>26</v>
       </c>
-      <c r="B172" s="79"/>
+      <c r="B172" s="72"/>
       <c r="C172" s="28" t="s">
         <v>40</v>
       </c>
@@ -23408,7 +24376,7 @@
       <c r="A173" s="26">
         <v>27</v>
       </c>
-      <c r="B173" s="80" t="s">
+      <c r="B173" s="71" t="s">
         <v>7</v>
       </c>
       <c r="C173" s="28" t="s">
@@ -23432,7 +24400,7 @@
       <c r="A174" s="26">
         <v>28</v>
       </c>
-      <c r="B174" s="79"/>
+      <c r="B174" s="72"/>
       <c r="C174" s="27" t="s">
         <v>175</v>
       </c>
@@ -23454,7 +24422,7 @@
       <c r="A175" s="26">
         <v>29</v>
       </c>
-      <c r="B175" s="79"/>
+      <c r="B175" s="72"/>
       <c r="C175" s="28" t="s">
         <v>178</v>
       </c>
@@ -23476,7 +24444,7 @@
       <c r="A176" s="26">
         <v>30</v>
       </c>
-      <c r="B176" s="89" t="s">
+      <c r="B176" s="76" t="s">
         <v>8</v>
       </c>
       <c r="C176" s="28" t="s">
@@ -23502,7 +24470,7 @@
       <c r="A177" s="31">
         <v>31</v>
       </c>
-      <c r="B177" s="90"/>
+      <c r="B177" s="77"/>
       <c r="C177" s="32" t="s">
         <v>183</v>
       </c>
@@ -23526,7 +24494,7 @@
       <c r="A178" s="23">
         <v>32</v>
       </c>
-      <c r="B178" s="91" t="s">
+      <c r="B178" s="80" t="s">
         <v>185</v>
       </c>
       <c r="C178" s="33" t="s">
@@ -23550,7 +24518,7 @@
       <c r="A179" s="26">
         <v>33</v>
       </c>
-      <c r="B179" s="92"/>
+      <c r="B179" s="81"/>
       <c r="C179" s="27" t="s">
         <v>189</v>
       </c>
@@ -23572,7 +24540,7 @@
       <c r="A180" s="26">
         <v>34</v>
       </c>
-      <c r="B180" s="93"/>
+      <c r="B180" s="82"/>
       <c r="C180" s="34" t="s">
         <v>192</v>
       </c>
@@ -23594,7 +24562,7 @@
       <c r="A181" s="31">
         <v>35</v>
       </c>
-      <c r="B181" s="93"/>
+      <c r="B181" s="82"/>
       <c r="C181" s="34" t="s">
         <v>193</v>
       </c>
@@ -23616,7 +24584,7 @@
       <c r="A182" s="31">
         <v>36</v>
       </c>
-      <c r="B182" s="93"/>
+      <c r="B182" s="82"/>
       <c r="C182" s="34" t="s">
         <v>196</v>
       </c>
@@ -23636,7 +24604,7 @@
       <c r="A183" s="31">
         <v>37</v>
       </c>
-      <c r="B183" s="93"/>
+      <c r="B183" s="82"/>
       <c r="C183" s="34" t="s">
         <v>248</v>
       </c>
@@ -23658,7 +24626,7 @@
       <c r="A184" s="35">
         <v>38</v>
       </c>
-      <c r="B184" s="88"/>
+      <c r="B184" s="83"/>
       <c r="C184" s="36" t="s">
         <v>252</v>
       </c>
@@ -23709,11 +24677,11 @@
       <c r="B198" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="C198" s="94" t="s">
+      <c r="C198" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="D198" s="94"/>
-      <c r="E198" s="94"/>
+      <c r="D198" s="84"/>
+      <c r="E198" s="84"/>
       <c r="F198" s="39" t="s">
         <v>42</v>
       </c>
@@ -23722,17 +24690,17 @@
       </c>
     </row>
     <row r="199" spans="1:7">
-      <c r="A199" s="77" t="s">
+      <c r="A199" s="85" t="s">
         <v>206</v>
       </c>
-      <c r="B199" s="79" t="s">
+      <c r="B199" s="72" t="s">
         <v>207</v>
       </c>
-      <c r="C199" s="96" t="s">
+      <c r="C199" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="D199" s="97"/>
-      <c r="E199" s="97"/>
+      <c r="D199" s="88"/>
+      <c r="E199" s="88"/>
       <c r="F199" s="28" t="s">
         <v>208</v>
       </c>
@@ -23741,13 +24709,13 @@
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="77"/>
-      <c r="B200" s="95"/>
-      <c r="C200" s="98" t="s">
+      <c r="A200" s="85"/>
+      <c r="B200" s="86"/>
+      <c r="C200" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="D200" s="99"/>
-      <c r="E200" s="99"/>
+      <c r="D200" s="90"/>
+      <c r="E200" s="90"/>
       <c r="F200" s="32" t="s">
         <v>209</v>
       </c>
@@ -23756,15 +24724,15 @@
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="77"/>
-      <c r="B201" s="79" t="s">
+      <c r="A201" s="85"/>
+      <c r="B201" s="72" t="s">
         <v>210</v>
       </c>
-      <c r="C201" s="100" t="s">
+      <c r="C201" s="91" t="s">
         <v>211</v>
       </c>
-      <c r="D201" s="100"/>
-      <c r="E201" s="100"/>
+      <c r="D201" s="91"/>
+      <c r="E201" s="91"/>
       <c r="F201" s="28" t="s">
         <v>208</v>
       </c>
@@ -23773,13 +24741,13 @@
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="77"/>
-      <c r="B202" s="79"/>
-      <c r="C202" s="98" t="s">
+      <c r="A202" s="85"/>
+      <c r="B202" s="72"/>
+      <c r="C202" s="89" t="s">
         <v>211</v>
       </c>
-      <c r="D202" s="98"/>
-      <c r="E202" s="98"/>
+      <c r="D202" s="89"/>
+      <c r="E202" s="89"/>
       <c r="F202" s="28" t="s">
         <v>209</v>
       </c>
@@ -23788,15 +24756,15 @@
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="77"/>
-      <c r="B203" s="95" t="s">
+      <c r="A203" s="85"/>
+      <c r="B203" s="86" t="s">
         <v>212</v>
       </c>
-      <c r="C203" s="101" t="s">
+      <c r="C203" s="92" t="s">
         <v>56</v>
       </c>
-      <c r="D203" s="102"/>
-      <c r="E203" s="103"/>
+      <c r="D203" s="93"/>
+      <c r="E203" s="94"/>
       <c r="F203" s="28" t="s">
         <v>208</v>
       </c>
@@ -23805,13 +24773,13 @@
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="77"/>
-      <c r="B204" s="84"/>
-      <c r="C204" s="101" t="s">
+      <c r="A204" s="85"/>
+      <c r="B204" s="78"/>
+      <c r="C204" s="92" t="s">
         <v>56</v>
       </c>
-      <c r="D204" s="102"/>
-      <c r="E204" s="103"/>
+      <c r="D204" s="93"/>
+      <c r="E204" s="94"/>
       <c r="F204" s="28" t="s">
         <v>209</v>
       </c>
@@ -23820,15 +24788,15 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="77"/>
-      <c r="B205" s="79" t="s">
+      <c r="A205" s="85"/>
+      <c r="B205" s="72" t="s">
         <v>213</v>
       </c>
-      <c r="C205" s="100" t="s">
+      <c r="C205" s="91" t="s">
         <v>214</v>
       </c>
-      <c r="D205" s="100"/>
-      <c r="E205" s="100"/>
+      <c r="D205" s="91"/>
+      <c r="E205" s="91"/>
       <c r="F205" s="28" t="s">
         <v>208</v>
       </c>
@@ -23837,13 +24805,13 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="77"/>
-      <c r="B206" s="79"/>
-      <c r="C206" s="100" t="s">
+      <c r="A206" s="85"/>
+      <c r="B206" s="72"/>
+      <c r="C206" s="91" t="s">
         <v>214</v>
       </c>
-      <c r="D206" s="100"/>
-      <c r="E206" s="100"/>
+      <c r="D206" s="91"/>
+      <c r="E206" s="91"/>
       <c r="F206" s="28" t="s">
         <v>209</v>
       </c>
@@ -23852,17 +24820,17 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="77" t="s">
+      <c r="A207" s="85" t="s">
         <v>215</v>
       </c>
-      <c r="B207" s="79" t="s">
+      <c r="B207" s="72" t="s">
         <v>216</v>
       </c>
-      <c r="C207" s="80" t="s">
+      <c r="C207" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="D207" s="79"/>
-      <c r="E207" s="79"/>
+      <c r="D207" s="72"/>
+      <c r="E207" s="72"/>
       <c r="F207" s="28" t="s">
         <v>208</v>
       </c>
@@ -23871,13 +24839,13 @@
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="77"/>
-      <c r="B208" s="79"/>
-      <c r="C208" s="79" t="s">
+      <c r="A208" s="85"/>
+      <c r="B208" s="72"/>
+      <c r="C208" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="D208" s="79"/>
-      <c r="E208" s="79"/>
+      <c r="D208" s="72"/>
+      <c r="E208" s="72"/>
       <c r="F208" s="28" t="s">
         <v>209</v>
       </c>
@@ -23886,15 +24854,15 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="77"/>
-      <c r="B209" s="79" t="s">
+      <c r="A209" s="85"/>
+      <c r="B209" s="72" t="s">
         <v>218</v>
       </c>
-      <c r="C209" s="79" t="s">
+      <c r="C209" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="D209" s="79"/>
-      <c r="E209" s="79"/>
+      <c r="D209" s="72"/>
+      <c r="E209" s="72"/>
       <c r="F209" s="28" t="s">
         <v>208</v>
       </c>
@@ -23903,13 +24871,13 @@
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="77"/>
-      <c r="B210" s="79"/>
-      <c r="C210" s="79" t="s">
+      <c r="A210" s="85"/>
+      <c r="B210" s="72"/>
+      <c r="C210" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="D210" s="79"/>
-      <c r="E210" s="79"/>
+      <c r="D210" s="72"/>
+      <c r="E210" s="72"/>
       <c r="F210" s="28" t="s">
         <v>209</v>
       </c>
@@ -23918,17 +24886,17 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="77" t="s">
+      <c r="A211" s="85" t="s">
         <v>219</v>
       </c>
-      <c r="B211" s="79" t="s">
+      <c r="B211" s="72" t="s">
         <v>220</v>
       </c>
-      <c r="C211" s="80" t="s">
+      <c r="C211" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="D211" s="79"/>
-      <c r="E211" s="79"/>
+      <c r="D211" s="72"/>
+      <c r="E211" s="72"/>
       <c r="F211" s="28" t="s">
         <v>208</v>
       </c>
@@ -23937,13 +24905,13 @@
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="77"/>
-      <c r="B212" s="79"/>
-      <c r="C212" s="79" t="s">
+      <c r="A212" s="85"/>
+      <c r="B212" s="72"/>
+      <c r="C212" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="D212" s="79"/>
-      <c r="E212" s="79"/>
+      <c r="D212" s="72"/>
+      <c r="E212" s="72"/>
       <c r="F212" s="28" t="s">
         <v>209</v>
       </c>
@@ -23952,15 +24920,15 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="77"/>
-      <c r="B213" s="79" t="s">
+      <c r="A213" s="85"/>
+      <c r="B213" s="72" t="s">
         <v>221</v>
       </c>
-      <c r="C213" s="80" t="s">
+      <c r="C213" s="71" t="s">
         <v>222</v>
       </c>
-      <c r="D213" s="79"/>
-      <c r="E213" s="79"/>
+      <c r="D213" s="72"/>
+      <c r="E213" s="72"/>
       <c r="F213" s="28" t="s">
         <v>208</v>
       </c>
@@ -23969,13 +24937,13 @@
       </c>
     </row>
     <row r="214" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A214" s="78"/>
-      <c r="B214" s="81"/>
-      <c r="C214" s="81" t="s">
+      <c r="A214" s="96"/>
+      <c r="B214" s="97"/>
+      <c r="C214" s="97" t="s">
         <v>223</v>
       </c>
-      <c r="D214" s="81"/>
-      <c r="E214" s="81"/>
+      <c r="D214" s="97"/>
+      <c r="E214" s="97"/>
       <c r="F214" s="36" t="s">
         <v>209</v>
       </c>
@@ -24014,12 +24982,12 @@
       <c r="A219" s="45" t="s">
         <v>226</v>
       </c>
-      <c r="B219" s="82" t="s">
+      <c r="B219" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="C219" s="82"/>
-      <c r="D219" s="82"/>
-      <c r="E219" s="82"/>
+      <c r="C219" s="98"/>
+      <c r="D219" s="98"/>
+      <c r="E219" s="98"/>
       <c r="F219" s="46" t="s">
         <v>227</v>
       </c>
@@ -24031,12 +24999,12 @@
       <c r="A220" s="48" t="s">
         <v>229</v>
       </c>
-      <c r="B220" s="83" t="s">
+      <c r="B220" s="99" t="s">
         <v>230</v>
       </c>
-      <c r="C220" s="84"/>
-      <c r="D220" s="84"/>
-      <c r="E220" s="84"/>
+      <c r="C220" s="78"/>
+      <c r="D220" s="78"/>
+      <c r="E220" s="78"/>
       <c r="F220" s="49" t="s">
         <v>105</v>
       </c>
@@ -24048,12 +25016,12 @@
       <c r="A221" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="B221" s="85" t="s">
+      <c r="B221" s="100" t="s">
         <v>232</v>
       </c>
-      <c r="C221" s="86"/>
-      <c r="D221" s="86"/>
-      <c r="E221" s="87"/>
+      <c r="C221" s="101"/>
+      <c r="D221" s="101"/>
+      <c r="E221" s="102"/>
       <c r="F221" s="15" t="s">
         <v>62</v>
       </c>
@@ -24065,12 +25033,12 @@
       <c r="A222" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B222" s="85" t="s">
+      <c r="B222" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="C222" s="86"/>
-      <c r="D222" s="86"/>
-      <c r="E222" s="87"/>
+      <c r="C222" s="101"/>
+      <c r="D222" s="101"/>
+      <c r="E222" s="102"/>
       <c r="F222" s="18" t="s">
         <v>62</v>
       </c>
@@ -24082,12 +25050,12 @@
       <c r="A223" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="B223" s="88" t="s">
+      <c r="B223" s="83" t="s">
         <v>235</v>
       </c>
-      <c r="C223" s="81"/>
-      <c r="D223" s="81"/>
-      <c r="E223" s="81"/>
+      <c r="C223" s="97"/>
+      <c r="D223" s="97"/>
+      <c r="E223" s="97"/>
       <c r="F223" s="21" t="s">
         <v>62</v>
       </c>
@@ -24132,11 +25100,11 @@
       <c r="C228" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D228" s="76" t="s">
+      <c r="D228" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="E228" s="76"/>
-      <c r="F228" s="76"/>
+      <c r="E228" s="95"/>
+      <c r="F228" s="95"/>
       <c r="G228" s="57"/>
     </row>
     <row r="229" spans="1:7">
@@ -24149,11 +25117,11 @@
       <c r="C229" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D229" s="75" t="s">
+      <c r="D229" s="107" t="s">
         <v>54</v>
       </c>
-      <c r="E229" s="75"/>
-      <c r="F229" s="75"/>
+      <c r="E229" s="107"/>
+      <c r="F229" s="107"/>
       <c r="G229" s="41"/>
     </row>
     <row r="230" spans="1:7">
@@ -24166,11 +25134,11 @@
       <c r="C230" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D230" s="75" t="s">
+      <c r="D230" s="107" t="s">
         <v>239</v>
       </c>
-      <c r="E230" s="75"/>
-      <c r="F230" s="75"/>
+      <c r="E230" s="107"/>
+      <c r="F230" s="107"/>
       <c r="G230" s="41"/>
     </row>
     <row r="231" spans="1:7">
@@ -24183,11 +25151,11 @@
       <c r="C231" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D231" s="75" t="s">
+      <c r="D231" s="107" t="s">
         <v>240</v>
       </c>
-      <c r="E231" s="75"/>
-      <c r="F231" s="75"/>
+      <c r="E231" s="107"/>
+      <c r="F231" s="107"/>
       <c r="G231" s="41"/>
     </row>
     <row r="232" spans="1:7">
@@ -24200,11 +25168,11 @@
       <c r="C232" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D232" s="75" t="s">
+      <c r="D232" s="107" t="s">
         <v>241</v>
       </c>
-      <c r="E232" s="75"/>
-      <c r="F232" s="75"/>
+      <c r="E232" s="107"/>
+      <c r="F232" s="107"/>
       <c r="G232" s="41"/>
     </row>
     <row r="233" spans="1:7">
@@ -24217,11 +25185,11 @@
       <c r="C233" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D233" s="75" t="s">
+      <c r="D233" s="107" t="s">
         <v>242</v>
       </c>
-      <c r="E233" s="75"/>
-      <c r="F233" s="75"/>
+      <c r="E233" s="107"/>
+      <c r="F233" s="107"/>
       <c r="G233" s="41"/>
     </row>
     <row r="234" spans="1:7">
@@ -24234,11 +25202,11 @@
       <c r="C234" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D234" s="71" t="s">
+      <c r="D234" s="103" t="s">
         <v>63</v>
       </c>
-      <c r="E234" s="72"/>
-      <c r="F234" s="73"/>
+      <c r="E234" s="104"/>
+      <c r="F234" s="105"/>
       <c r="G234" s="43"/>
     </row>
     <row r="235" spans="1:7">
@@ -24251,11 +25219,11 @@
       <c r="C235" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D235" s="71" t="s">
+      <c r="D235" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="E235" s="72"/>
-      <c r="F235" s="73"/>
+      <c r="E235" s="104"/>
+      <c r="F235" s="105"/>
       <c r="G235" s="43"/>
     </row>
     <row r="236" spans="1:7">
@@ -24268,11 +25236,11 @@
       <c r="C236" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D236" s="71" t="s">
+      <c r="D236" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="E236" s="72"/>
-      <c r="F236" s="73"/>
+      <c r="E236" s="104"/>
+      <c r="F236" s="105"/>
       <c r="G236" s="43"/>
     </row>
     <row r="237" spans="1:7">
@@ -24353,11 +25321,11 @@
       <c r="C241" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="D241" s="74" t="s">
+      <c r="D241" s="106" t="s">
         <v>255</v>
       </c>
-      <c r="E241" s="74"/>
-      <c r="F241" s="74"/>
+      <c r="E241" s="106"/>
+      <c r="F241" s="106"/>
       <c r="G241" s="44"/>
     </row>
   </sheetData>
@@ -24374,12 +25342,35 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="B173:B175"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B147:B159"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="B165:B172"/>
+    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D241:F241"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D228:F228"/>
+    <mergeCell ref="A211:A214"/>
+    <mergeCell ref="B211:B212"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="B213:B214"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="B219:E219"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="A207:A210"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="B209:B210"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
     <mergeCell ref="B176:B177"/>
     <mergeCell ref="B178:B184"/>
     <mergeCell ref="C198:E198"/>
@@ -24396,35 +25387,12 @@
     <mergeCell ref="B205:B206"/>
     <mergeCell ref="C205:E205"/>
     <mergeCell ref="C206:E206"/>
-    <mergeCell ref="A207:A210"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="C207:E207"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="B209:B210"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="D228:F228"/>
-    <mergeCell ref="A211:A214"/>
-    <mergeCell ref="B211:B212"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="B213:B214"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="B219:E219"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D241:F241"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="B173:B175"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B147:B159"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="B162:B164"/>
+    <mergeCell ref="B165:B172"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -24450,15 +25418,15 @@
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i479--EIT2 suite remove ignore case
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_04_jedi.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_04_jedi.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{5DF25FC7-3CE5-460C-B8E1-871B1CE9E034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BBPw5sjxCCUVqKqDFh1VvlGl+6jBsyEv58ubpDIjFduKT4EttifNtZLgNn2j4jGi/bvDsFNRyO0+XWiClC3JHw==" workbookSaltValue="FQsz7bLsuDdqgfH6Nya7QA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -27,16 +28,16 @@
   </definedNames>
   <calcPr calcId="122211" calcOnSave="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="390">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -858,9 +859,6 @@
     <t>=sim</t>
   </si>
   <si>
-    <t>Quin.Xu</t>
-  </si>
-  <si>
     <t>repository =http://lsh-tmp/radiant/trunk/silicon/00_basic</t>
   </si>
   <si>
@@ -1152,9 +1150,6 @@
     <t>00_primitive/06_DDR/11_IDDRX2_12_gddrx2</t>
   </si>
   <si>
-    <t>00_primitive/06_DDR/13_IDDRX4_16_gddrx4</t>
-  </si>
-  <si>
     <t>00_primitive/06_DDR/15_IDDRX5_17_gddrx5</t>
   </si>
   <si>
@@ -1170,9 +1165,6 @@
     <t>00_primitive/06_DDR/25_OSHX2_31_mddrx2_oshx2</t>
   </si>
   <si>
-    <t>00_primitive/06_DDR/26_OSHX4_31_mddrx4_oshx4</t>
-  </si>
-  <si>
     <t>00_primitive/07_Misc/00_ADC</t>
   </si>
   <si>
@@ -1243,12 +1235,15 @@
   </si>
   <si>
     <t>radiant=ng3_0</t>
+  </si>
+  <si>
+    <t>Jason.Wang</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00_ "/>
     <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
@@ -2333,7 +2328,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2341,13 +2336,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="47">
@@ -2407,7 +2402,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2443,22 +2438,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="47" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="36" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="41" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2488,22 +2474,16 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="49" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="15" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="21" fillId="0" borderId="16" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2518,13 +2498,13 @@
     <xf numFmtId="165" fontId="21" fillId="0" borderId="24" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="21" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2545,31 +2525,64 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2581,13 +2594,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2607,44 +2614,17 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -2681,19 +2661,19 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink 2" xfId="49"/>
+    <cellStyle name="Hyperlink 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="41"/>
-    <cellStyle name="Normal 2 2" xfId="47"/>
-    <cellStyle name="Normal 3" xfId="44"/>
-    <cellStyle name="Normal 4" xfId="45"/>
-    <cellStyle name="Normal 5" xfId="46"/>
-    <cellStyle name="Normal 6" xfId="43"/>
-    <cellStyle name="Normal 6 2" xfId="48"/>
-    <cellStyle name="Note 2" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 4" xfId="45" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 5" xfId="46" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 6" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 6 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Note 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
@@ -2729,7 +2709,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4845,7 +4831,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -4900,7 +4892,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4945,7 +4943,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5064,7 +5068,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5111,7 +5121,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5147,7 +5163,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F2C20D40-0E95-4DF4-B22D-E0617ADAE023}" diskRevisions="1" revisionId="1532" version="29">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0AF23792-2803-4DFD-B32E-BC59B929B60B}" diskRevisions="1" revisionId="1558" version="31">
   <header guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" dateTime="2020-10-15T13:42:26" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5380,6 +5396,22 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{B97CC043-F570-4096-8828-91F299071B03}" dateTime="2023-10-11T19:20:40" maxSheetId="5" userName="Jason Wang" r:id="rId30" minRId="1533" maxRId="1557">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0AF23792-2803-4DFD-B32E-BC59B929B60B}" dateTime="2023-10-11T19:20:54" maxSheetId="5" userName="Jason Wang" r:id="rId31" minRId="1558">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -12726,6 +12758,290 @@
     <oldFormula>case!$A$2:$AD$2</oldFormula>
   </rdn>
   <rcv guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog30.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="1533" sId="2" ref="A92:XFD92" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A92:XFD92" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="30" formatCode="@"/>
+        <protection locked="0"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2" numFmtId="30">
+      <nc r="A92">
+        <v>90</v>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="E92" t="inlineStr">
+        <is>
+          <t>00_primitive/06_DDR/13_IDDRX4_16_gddrx4</t>
+        </is>
+      </nc>
+    </rcc>
+    <rfmt sheetId="2" sqref="L92" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="0" formatCode="General"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="S92" t="inlineStr">
+        <is>
+          <t>primitive</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="AD92" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rrc rId="1534" sId="2" ref="A97:XFD97" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A97:XFD97" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="30" formatCode="@"/>
+        <protection locked="0"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2" numFmtId="30">
+      <nc r="A97">
+        <v>96</v>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="E97" t="inlineStr">
+        <is>
+          <t>00_primitive/06_DDR/26_OSHX4_31_mddrx4_oshx4</t>
+        </is>
+      </nc>
+    </rcc>
+    <rfmt sheetId="2" sqref="L97" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="0" formatCode="General"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="S97" t="inlineStr">
+        <is>
+          <t>primitive</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="AD97" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rcc rId="1535" sId="2" numFmtId="30">
+    <oc r="A92">
+      <v>91</v>
+    </oc>
+    <nc r="A92">
+      <v>90</v>
+    </nc>
+  </rcc>
+  <rcc rId="1536" sId="2" numFmtId="30">
+    <oc r="A93">
+      <v>92</v>
+    </oc>
+    <nc r="A93">
+      <v>91</v>
+    </nc>
+  </rcc>
+  <rcc rId="1537" sId="2" numFmtId="30">
+    <oc r="A94">
+      <v>93</v>
+    </oc>
+    <nc r="A94">
+      <v>92</v>
+    </nc>
+  </rcc>
+  <rcc rId="1538" sId="2" numFmtId="30">
+    <oc r="A95">
+      <v>94</v>
+    </oc>
+    <nc r="A95">
+      <v>93</v>
+    </nc>
+  </rcc>
+  <rcc rId="1539" sId="2" numFmtId="30">
+    <oc r="A96">
+      <v>95</v>
+    </oc>
+    <nc r="A96">
+      <v>94</v>
+    </nc>
+  </rcc>
+  <rcc rId="1540" sId="2" numFmtId="30">
+    <oc r="A97">
+      <v>97</v>
+    </oc>
+    <nc r="A97">
+      <v>95</v>
+    </nc>
+  </rcc>
+  <rcc rId="1541" sId="2" numFmtId="30">
+    <oc r="A98">
+      <v>98</v>
+    </oc>
+    <nc r="A98">
+      <v>96</v>
+    </nc>
+  </rcc>
+  <rcc rId="1542" sId="2" numFmtId="30">
+    <oc r="A99">
+      <v>99</v>
+    </oc>
+    <nc r="A99">
+      <v>97</v>
+    </nc>
+  </rcc>
+  <rcc rId="1543" sId="2" numFmtId="30">
+    <oc r="A100">
+      <v>100</v>
+    </oc>
+    <nc r="A100">
+      <v>98</v>
+    </nc>
+  </rcc>
+  <rcc rId="1544" sId="2" numFmtId="30">
+    <oc r="A101">
+      <v>101</v>
+    </oc>
+    <nc r="A101">
+      <v>99</v>
+    </nc>
+  </rcc>
+  <rcc rId="1545" sId="2" numFmtId="30">
+    <oc r="A102">
+      <v>102</v>
+    </oc>
+    <nc r="A102">
+      <v>100</v>
+    </nc>
+  </rcc>
+  <rcc rId="1546" sId="2" numFmtId="30">
+    <oc r="A103">
+      <v>103</v>
+    </oc>
+    <nc r="A103">
+      <v>101</v>
+    </nc>
+  </rcc>
+  <rcc rId="1547" sId="2" numFmtId="30">
+    <oc r="A104">
+      <v>104</v>
+    </oc>
+    <nc r="A104">
+      <v>102</v>
+    </nc>
+  </rcc>
+  <rcc rId="1548" sId="2" numFmtId="30">
+    <oc r="A105">
+      <v>105</v>
+    </oc>
+    <nc r="A105">
+      <v>103</v>
+    </nc>
+  </rcc>
+  <rcc rId="1549" sId="2" numFmtId="30">
+    <oc r="A106">
+      <v>106</v>
+    </oc>
+    <nc r="A106">
+      <v>104</v>
+    </nc>
+  </rcc>
+  <rcc rId="1550" sId="2" numFmtId="30">
+    <oc r="A107">
+      <v>107</v>
+    </oc>
+    <nc r="A107">
+      <v>105</v>
+    </nc>
+  </rcc>
+  <rcc rId="1551" sId="2" numFmtId="30">
+    <oc r="A108">
+      <v>108</v>
+    </oc>
+    <nc r="A108">
+      <v>106</v>
+    </nc>
+  </rcc>
+  <rcc rId="1552" sId="2" numFmtId="30">
+    <oc r="A109">
+      <v>109</v>
+    </oc>
+    <nc r="A109">
+      <v>107</v>
+    </nc>
+  </rcc>
+  <rcc rId="1553" sId="2" numFmtId="30">
+    <oc r="A110">
+      <v>110</v>
+    </oc>
+    <nc r="A110">
+      <v>108</v>
+    </nc>
+  </rcc>
+  <rcc rId="1554" sId="2" numFmtId="30">
+    <oc r="A111">
+      <v>111</v>
+    </oc>
+    <nc r="A111">
+      <v>109</v>
+    </nc>
+  </rcc>
+  <rcc rId="1555" sId="2" numFmtId="30">
+    <oc r="A112">
+      <v>112</v>
+    </oc>
+    <nc r="A112">
+      <v>110</v>
+    </nc>
+  </rcc>
+  <rcc rId="1556" sId="2" numFmtId="30">
+    <oc r="A113">
+      <v>113</v>
+    </oc>
+    <nc r="A113">
+      <v>111</v>
+    </nc>
+  </rcc>
+  <rcc rId="1557" sId="2" numFmtId="30">
+    <oc r="A114">
+      <v>114</v>
+    </oc>
+    <nc r="A114">
+      <v>112</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog31.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1558" sId="1">
+    <oc r="B1" t="inlineStr">
+      <is>
+        <t>Quin.Xu</t>
+      </is>
+    </oc>
+    <nc r="B1" t="inlineStr">
+      <is>
+        <t>Jason.Wang</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -20471,16 +20787,16 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
   <userInfo guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" name="Cherry (Ying) Xu" id="-707422276" dateTime="2020-11-23T15:52:35"/>
 </users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -20518,9 +20834,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -20555,7 +20871,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -20590,7 +20906,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -20763,11 +21079,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -20782,7 +21098,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>263</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -20798,7 +21114,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -20806,12 +21122,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -20824,7 +21140,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -20832,7 +21148,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -20869,7 +21185,7 @@
         <v>108</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -20880,7 +21196,7 @@
         <v>87</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -20891,7 +21207,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -20918,7 +21234,7 @@
         <v>108</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -20929,7 +21245,7 @@
         <v>87</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -20940,7 +21256,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -20951,23 +21267,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B27" sqref="B27"/>
+    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}">
+      <selection activeCell="C37" sqref="C37"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}">
-      <selection activeCell="C37" sqref="C37"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B27" sqref="B27"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -20979,15 +21295,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD116"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AD114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B116" sqref="B116"/>
+      <selection pane="bottomRight" activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -21020,40 +21336,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="70" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
     </row>
     <row r="2" spans="1:30" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -21152,13 +21468,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -21166,13 +21482,13 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -21180,10 +21496,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD5" s="2" t="s">
         <v>261</v>
@@ -21194,13 +21510,13 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -21208,13 +21524,13 @@
         <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -21222,13 +21538,13 @@
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -21236,13 +21552,13 @@
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -21250,13 +21566,13 @@
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -21264,13 +21580,13 @@
         <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -21278,13 +21594,13 @@
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -21292,13 +21608,13 @@
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:30">
@@ -21306,13 +21622,13 @@
         <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="15" spans="1:30">
@@ -21320,13 +21636,13 @@
         <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -21334,13 +21650,13 @@
         <v>14</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD16" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="17" spans="1:30">
@@ -21348,13 +21664,13 @@
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:30">
@@ -21362,13 +21678,13 @@
         <v>16</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD18" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="19" spans="1:30">
@@ -21376,13 +21692,13 @@
         <v>17</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="20" spans="1:30">
@@ -21390,13 +21706,13 @@
         <v>18</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD20" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="21" spans="1:30">
@@ -21404,13 +21720,13 @@
         <v>19</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="22" spans="1:30">
@@ -21418,10 +21734,10 @@
         <v>20</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD22" s="2" t="s">
         <v>261</v>
@@ -21432,13 +21748,13 @@
         <v>21</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD23" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="24" spans="1:30">
@@ -21446,10 +21762,10 @@
         <v>22</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD24" s="2" t="s">
         <v>261</v>
@@ -21460,10 +21776,10 @@
         <v>23</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD25" s="2" t="s">
         <v>261</v>
@@ -21474,10 +21790,10 @@
         <v>24</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD26" s="2" t="s">
         <v>261</v>
@@ -21488,10 +21804,10 @@
         <v>25</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD27" s="2" t="s">
         <v>261</v>
@@ -21502,10 +21818,10 @@
         <v>26</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD28" s="2" t="s">
         <v>261</v>
@@ -21516,13 +21832,13 @@
         <v>27</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD29" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="30" spans="1:30">
@@ -21530,10 +21846,10 @@
         <v>28</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD30" s="2" t="s">
         <v>261</v>
@@ -21544,13 +21860,13 @@
         <v>29</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD31" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="32" spans="1:30">
@@ -21558,13 +21874,13 @@
         <v>30</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD32" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="33" spans="1:30">
@@ -21572,16 +21888,16 @@
         <v>31</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="O33" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="O33" s="2" t="s">
-        <v>302</v>
-      </c>
       <c r="S33" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD33" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="34" spans="1:30">
@@ -21589,13 +21905,13 @@
         <v>32</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD34" s="2" t="s">
         <v>261</v>
@@ -21606,13 +21922,13 @@
         <v>33</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD35" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="36" spans="1:30">
@@ -21620,13 +21936,13 @@
         <v>34</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD36" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="37" spans="1:30">
@@ -21634,13 +21950,13 @@
         <v>35</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD37" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="38" spans="1:30">
@@ -21648,13 +21964,13 @@
         <v>36</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD38" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="39" spans="1:30">
@@ -21662,10 +21978,10 @@
         <v>37</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD39" s="2" t="s">
         <v>261</v>
@@ -21676,13 +21992,13 @@
         <v>38</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD40" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="41" spans="1:30">
@@ -21690,13 +22006,13 @@
         <v>39</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD41" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="42" spans="1:30">
@@ -21704,13 +22020,13 @@
         <v>40</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD42" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="43" spans="1:30">
@@ -21718,13 +22034,13 @@
         <v>41</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD43" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="44" spans="1:30">
@@ -21732,13 +22048,13 @@
         <v>42</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD44" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="45" spans="1:30">
@@ -21746,13 +22062,13 @@
         <v>43</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD45" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="46" spans="1:30">
@@ -21760,13 +22076,13 @@
         <v>44</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD46" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="47" spans="1:30">
@@ -21774,13 +22090,13 @@
         <v>45</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD47" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="48" spans="1:30">
@@ -21788,13 +22104,13 @@
         <v>46</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD48" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="49" spans="1:30">
@@ -21802,13 +22118,13 @@
         <v>47</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD49" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="50" spans="1:30">
@@ -21816,13 +22132,13 @@
         <v>48</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD50" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="51" spans="1:30">
@@ -21830,13 +22146,13 @@
         <v>49</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD51" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="52" spans="1:30">
@@ -21844,13 +22160,13 @@
         <v>50</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="S52" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD52" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="53" spans="1:30">
@@ -21858,13 +22174,13 @@
         <v>51</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="S53" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD53" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="54" spans="1:30">
@@ -21872,13 +22188,13 @@
         <v>52</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="S54" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD54" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="55" spans="1:30">
@@ -21886,13 +22202,13 @@
         <v>53</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="S55" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD55" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="56" spans="1:30">
@@ -21900,13 +22216,13 @@
         <v>54</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="S56" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD56" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="57" spans="1:30">
@@ -21914,13 +22230,13 @@
         <v>55</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="S57" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD57" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="58" spans="1:30">
@@ -21928,13 +22244,13 @@
         <v>56</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S58" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD58" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="59" spans="1:30">
@@ -21942,13 +22258,13 @@
         <v>57</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="S59" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD59" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="60" spans="1:30">
@@ -21956,13 +22272,13 @@
         <v>58</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="S60" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD60" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="61" spans="1:30">
@@ -21970,13 +22286,13 @@
         <v>59</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="S61" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD61" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="62" spans="1:30">
@@ -21984,13 +22300,13 @@
         <v>60</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S62" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD62" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="63" spans="1:30">
@@ -21998,13 +22314,13 @@
         <v>61</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="S63" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD63" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="64" spans="1:30">
@@ -22012,13 +22328,13 @@
         <v>62</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="S64" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD64" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="65" spans="1:30">
@@ -22026,13 +22342,13 @@
         <v>63</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="S65" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD65" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="66" spans="1:30">
@@ -22040,13 +22356,13 @@
         <v>64</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="S66" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD66" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="67" spans="1:30">
@@ -22054,13 +22370,13 @@
         <v>65</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="S67" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD67" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="68" spans="1:30">
@@ -22068,13 +22384,13 @@
         <v>66</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S68" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD68" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="69" spans="1:30">
@@ -22082,13 +22398,13 @@
         <v>67</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="S69" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD69" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="70" spans="1:30">
@@ -22096,13 +22412,13 @@
         <v>68</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="S70" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD70" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="71" spans="1:30">
@@ -22110,10 +22426,10 @@
         <v>69</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="S71" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD71" s="2" t="s">
         <v>261</v>
@@ -22124,13 +22440,13 @@
         <v>70</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="S72" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD72" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="73" spans="1:30">
@@ -22138,13 +22454,13 @@
         <v>71</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="S73" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD73" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="74" spans="1:30">
@@ -22152,10 +22468,10 @@
         <v>72</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="S74" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD74" s="2" t="s">
         <v>261</v>
@@ -22166,13 +22482,13 @@
         <v>73</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="S75" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD75" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="76" spans="1:30">
@@ -22180,13 +22496,13 @@
         <v>74</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="S76" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD76" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="77" spans="1:30">
@@ -22194,13 +22510,13 @@
         <v>75</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S77" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD77" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="78" spans="1:30">
@@ -22208,13 +22524,13 @@
         <v>76</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="S78" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD78" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="79" spans="1:30">
@@ -22222,13 +22538,13 @@
         <v>77</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="S79" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD79" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="80" spans="1:30">
@@ -22236,13 +22552,13 @@
         <v>78</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="S80" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD80" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="81" spans="1:30">
@@ -22250,13 +22566,13 @@
         <v>79</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="S81" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD81" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="82" spans="1:30">
@@ -22264,10 +22580,10 @@
         <v>80</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="S82" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD82" s="2" t="s">
         <v>261</v>
@@ -22278,13 +22594,13 @@
         <v>81</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="S83" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD83" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="84" spans="1:30">
@@ -22292,10 +22608,10 @@
         <v>82</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S84" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD84" s="2" t="s">
         <v>261</v>
@@ -22306,13 +22622,13 @@
         <v>83</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="S85" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD85" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="86" spans="1:30">
@@ -22320,13 +22636,13 @@
         <v>84</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="S86" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD86" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="87" spans="1:30">
@@ -22334,13 +22650,13 @@
         <v>85</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S87" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD87" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="88" spans="1:30">
@@ -22348,13 +22664,13 @@
         <v>86</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="S88" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD88" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="89" spans="1:30">
@@ -22362,13 +22678,13 @@
         <v>87</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="S89" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD89" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="90" spans="1:30">
@@ -22376,13 +22692,13 @@
         <v>88</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S90" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD90" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="91" spans="1:30">
@@ -22390,13 +22706,13 @@
         <v>89</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="S91" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD91" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="92" spans="1:30">
@@ -22404,13 +22720,13 @@
         <v>90</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="S92" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD92" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="93" spans="1:30">
@@ -22418,13 +22734,13 @@
         <v>91</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="S93" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD93" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="94" spans="1:30">
@@ -22432,13 +22748,13 @@
         <v>92</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="S94" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD94" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="95" spans="1:30">
@@ -22446,13 +22762,13 @@
         <v>93</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S95" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD95" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="96" spans="1:30">
@@ -22460,13 +22776,13 @@
         <v>94</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="S96" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD96" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="97" spans="1:30">
@@ -22474,13 +22790,16 @@
         <v>95</v>
       </c>
       <c r="E97" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="O97" s="2" t="s">
         <v>366</v>
       </c>
       <c r="S97" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD97" s="2" t="s">
-        <v>388</v>
+        <v>261</v>
       </c>
     </row>
     <row r="98" spans="1:30">
@@ -22491,10 +22810,10 @@
         <v>367</v>
       </c>
       <c r="S98" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD98" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="99" spans="1:30">
@@ -22504,14 +22823,11 @@
       <c r="E99" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="O99" s="2" t="s">
-        <v>369</v>
-      </c>
       <c r="S99" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD99" s="2" t="s">
-        <v>261</v>
+        <v>385</v>
       </c>
     </row>
     <row r="100" spans="1:30">
@@ -22519,13 +22835,13 @@
         <v>98</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S100" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD100" s="2" t="s">
-        <v>388</v>
+        <v>261</v>
       </c>
     </row>
     <row r="101" spans="1:30">
@@ -22533,13 +22849,13 @@
         <v>99</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="S101" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD101" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="102" spans="1:30">
@@ -22547,13 +22863,13 @@
         <v>100</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="S102" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD102" s="2" t="s">
-        <v>261</v>
+        <v>385</v>
       </c>
     </row>
     <row r="103" spans="1:30">
@@ -22561,13 +22877,13 @@
         <v>101</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="S103" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD103" s="2" t="s">
-        <v>388</v>
+        <v>261</v>
       </c>
     </row>
     <row r="104" spans="1:30">
@@ -22575,13 +22891,13 @@
         <v>102</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S104" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD104" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="105" spans="1:30">
@@ -22589,13 +22905,13 @@
         <v>103</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S105" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD105" s="2" t="s">
-        <v>261</v>
+        <v>385</v>
       </c>
     </row>
     <row r="106" spans="1:30">
@@ -22603,13 +22919,13 @@
         <v>104</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="S106" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD106" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="107" spans="1:30">
@@ -22617,13 +22933,13 @@
         <v>105</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="S107" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD107" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="108" spans="1:30">
@@ -22631,13 +22947,13 @@
         <v>106</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="S108" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD108" s="2" t="s">
-        <v>388</v>
+        <v>261</v>
       </c>
     </row>
     <row r="109" spans="1:30">
@@ -22645,13 +22961,13 @@
         <v>107</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="S109" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD109" s="2" t="s">
-        <v>388</v>
+        <v>261</v>
       </c>
     </row>
     <row r="110" spans="1:30">
@@ -22659,13 +22975,13 @@
         <v>108</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="S110" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD110" s="2" t="s">
-        <v>261</v>
+        <v>385</v>
       </c>
     </row>
     <row r="111" spans="1:30">
@@ -22673,10 +22989,10 @@
         <v>109</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="S111" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD111" s="2" t="s">
         <v>261</v>
@@ -22687,13 +23003,13 @@
         <v>110</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="S112" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD112" s="2" t="s">
-        <v>388</v>
+        <v>261</v>
       </c>
     </row>
     <row r="113" spans="1:30">
@@ -22701,10 +23017,10 @@
         <v>111</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="S113" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AD113" s="2" t="s">
         <v>261</v>
@@ -22715,74 +23031,46 @@
         <v>112</v>
       </c>
       <c r="E114" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="S114" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="S114" s="2" t="s">
-        <v>387</v>
-      </c>
       <c r="AD114" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="115" spans="1:30">
-      <c r="A115" s="2">
-        <v>113</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="S115" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="AD115" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="116" spans="1:30">
-      <c r="A116" s="2">
-        <v>114</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="S116" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="AD116" s="2" t="s">
         <v>261</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="y+CBG6/YKaQ6HsaQYTqaGGAc9K7SdI4KYNN5n42I5k04yiTX0Fn8xQwrYnwNAtl9mwRmr3UcHPCrpySoPgBJNA==" saltValue="2QS/OSgjoJCpqDc5Ec8Idw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A2:AD2"/>
+  <autoFilter ref="A2:AD2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B116" sqref="B116"/>
+    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" scale="70" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="F87" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="O114" sqref="O114"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:AD2"/>
+      <autoFilter ref="A2:AD2" xr:uid="{3FE11130-1CCC-45F4-B900-CA4892397AE7}"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A2:Y2" xr:uid="{BD56282D-7EF1-48FE-80A0-25546DF1A1E1}"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A2:Y2"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+      <autoFilter ref="A2:Y2" xr:uid="{C6EE0AC2-197C-4D72-9F78-D0C2823AA5B9}"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:Y2"/>
-    </customSheetView>
-    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" scale="70" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="F87" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="O114" sqref="O114"/>
+      <selection pane="bottomRight" activeCell="B116" sqref="B116"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A2:AD2"/>
+      <autoFilter ref="A2:AD2" xr:uid="{F0104AC4-58A0-4A97-A72A-A401C8821E4E}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -22791,7 +23079,7 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1 M1:AA1 G1:H1 C1:E1 A1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1 M1:AA1 G1:H1 C1:E1 A1" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -22800,49 +23088,49 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>description!$F$140:$H$140</xm:f>
           </x14:formula1>
           <xm:sqref>AB1:AB1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>description!$F$141:$H$141</xm:f>
           </x14:formula1>
           <xm:sqref>AC1:AC1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>description!$F$122:$H$122</xm:f>
           </x14:formula1>
           <xm:sqref>K1:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>description!$F$121:$K$121</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>description!$F$123:$H$123</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>description!$E$113:$F$113</xm:f>
           </x14:formula1>
           <xm:sqref>B1:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>description!$F$117:$H$117</xm:f>
           </x14:formula1>
           <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>description!$F$120:$K$120</xm:f>
           </x14:formula1>
@@ -22855,7 +23143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N241"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
@@ -22918,17 +23206,17 @@
       <c r="E111" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F111" s="73" t="s">
+      <c r="F111" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="G111" s="74"/>
-      <c r="H111" s="74"/>
-      <c r="I111" s="74"/>
-      <c r="J111" s="74"/>
-      <c r="K111" s="74"/>
-      <c r="L111" s="74"/>
-      <c r="M111" s="74"/>
-      <c r="N111" s="75"/>
+      <c r="G111" s="100"/>
+      <c r="H111" s="100"/>
+      <c r="I111" s="100"/>
+      <c r="J111" s="100"/>
+      <c r="K111" s="100"/>
+      <c r="L111" s="100"/>
+      <c r="M111" s="100"/>
+      <c r="N111" s="101"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -23792,7 +24080,7 @@
       <c r="A147" s="26">
         <v>1</v>
       </c>
-      <c r="B147" s="76" t="s">
+      <c r="B147" s="84" t="s">
         <v>3</v>
       </c>
       <c r="C147" s="27" t="s">
@@ -23818,7 +24106,7 @@
       <c r="A148" s="26">
         <v>2</v>
       </c>
-      <c r="B148" s="77"/>
+      <c r="B148" s="85"/>
       <c r="C148" s="28" t="s">
         <v>130</v>
       </c>
@@ -23840,7 +24128,7 @@
       <c r="A149" s="26">
         <v>3</v>
       </c>
-      <c r="B149" s="77"/>
+      <c r="B149" s="85"/>
       <c r="C149" s="28" t="s">
         <v>9</v>
       </c>
@@ -23860,7 +24148,7 @@
       <c r="A150" s="26">
         <v>4</v>
       </c>
-      <c r="B150" s="77"/>
+      <c r="B150" s="85"/>
       <c r="C150" s="28" t="s">
         <v>132</v>
       </c>
@@ -23884,7 +24172,7 @@
       <c r="A151" s="26">
         <v>5</v>
       </c>
-      <c r="B151" s="77"/>
+      <c r="B151" s="85"/>
       <c r="C151" s="27" t="s">
         <v>134</v>
       </c>
@@ -23908,7 +24196,7 @@
       <c r="A152" s="26">
         <v>6</v>
       </c>
-      <c r="B152" s="77"/>
+      <c r="B152" s="85"/>
       <c r="C152" s="27" t="s">
         <v>138</v>
       </c>
@@ -23932,7 +24220,7 @@
       <c r="A153" s="26">
         <v>7</v>
       </c>
-      <c r="B153" s="77"/>
+      <c r="B153" s="85"/>
       <c r="C153" s="28" t="s">
         <v>141</v>
       </c>
@@ -23954,7 +24242,7 @@
       <c r="A154" s="26">
         <v>8</v>
       </c>
-      <c r="B154" s="77"/>
+      <c r="B154" s="85"/>
       <c r="C154" s="27" t="s">
         <v>142</v>
       </c>
@@ -23978,7 +24266,7 @@
       <c r="A155" s="26">
         <v>9</v>
       </c>
-      <c r="B155" s="77"/>
+      <c r="B155" s="85"/>
       <c r="C155" s="27" t="s">
         <v>143</v>
       </c>
@@ -24002,7 +24290,7 @@
       <c r="A156" s="26">
         <v>10</v>
       </c>
-      <c r="B156" s="77"/>
+      <c r="B156" s="85"/>
       <c r="C156" s="28" t="s">
         <v>144</v>
       </c>
@@ -24026,7 +24314,7 @@
       <c r="A157" s="26">
         <v>11</v>
       </c>
-      <c r="B157" s="77"/>
+      <c r="B157" s="85"/>
       <c r="C157" s="28" t="s">
         <v>145</v>
       </c>
@@ -24050,7 +24338,7 @@
       <c r="A158" s="26">
         <v>12</v>
       </c>
-      <c r="B158" s="77"/>
+      <c r="B158" s="85"/>
       <c r="C158" s="28" t="s">
         <v>147</v>
       </c>
@@ -24072,7 +24360,7 @@
       <c r="A159" s="26">
         <v>13</v>
       </c>
-      <c r="B159" s="78"/>
+      <c r="B159" s="79"/>
       <c r="C159" s="28" t="s">
         <v>55</v>
       </c>
@@ -24096,7 +24384,7 @@
       <c r="A160" s="26">
         <v>14</v>
       </c>
-      <c r="B160" s="71" t="s">
+      <c r="B160" s="75" t="s">
         <v>4</v>
       </c>
       <c r="C160" s="28" t="s">
@@ -24122,7 +24410,7 @@
       <c r="A161" s="26">
         <v>15</v>
       </c>
-      <c r="B161" s="72"/>
+      <c r="B161" s="74"/>
       <c r="C161" s="28" t="s">
         <v>155</v>
       </c>
@@ -24146,7 +24434,7 @@
       <c r="A162" s="26">
         <v>16</v>
       </c>
-      <c r="B162" s="76" t="s">
+      <c r="B162" s="84" t="s">
         <v>5</v>
       </c>
       <c r="C162" s="28" t="s">
@@ -24170,7 +24458,7 @@
       <c r="A163" s="26">
         <v>17</v>
       </c>
-      <c r="B163" s="79"/>
+      <c r="B163" s="102"/>
       <c r="C163" s="27" t="s">
         <v>159</v>
       </c>
@@ -24192,7 +24480,7 @@
       <c r="A164" s="26">
         <v>18</v>
       </c>
-      <c r="B164" s="78"/>
+      <c r="B164" s="79"/>
       <c r="C164" s="27" t="s">
         <v>161</v>
       </c>
@@ -24212,7 +24500,7 @@
       <c r="A165" s="26">
         <v>19</v>
       </c>
-      <c r="B165" s="71" t="s">
+      <c r="B165" s="75" t="s">
         <v>6</v>
       </c>
       <c r="C165" s="28" t="s">
@@ -24236,7 +24524,7 @@
       <c r="A166" s="26">
         <v>20</v>
       </c>
-      <c r="B166" s="72"/>
+      <c r="B166" s="74"/>
       <c r="C166" s="28" t="s">
         <v>166</v>
       </c>
@@ -24256,7 +24544,7 @@
       <c r="A167" s="26">
         <v>21</v>
       </c>
-      <c r="B167" s="72"/>
+      <c r="B167" s="74"/>
       <c r="C167" s="28" t="s">
         <v>167</v>
       </c>
@@ -24276,7 +24564,7 @@
       <c r="A168" s="26">
         <v>22</v>
       </c>
-      <c r="B168" s="72"/>
+      <c r="B168" s="74"/>
       <c r="C168" s="28" t="s">
         <v>168</v>
       </c>
@@ -24296,7 +24584,7 @@
       <c r="A169" s="26">
         <v>23</v>
       </c>
-      <c r="B169" s="72"/>
+      <c r="B169" s="74"/>
       <c r="C169" s="28" t="s">
         <v>169</v>
       </c>
@@ -24316,7 +24604,7 @@
       <c r="A170" s="26">
         <v>24</v>
       </c>
-      <c r="B170" s="72"/>
+      <c r="B170" s="74"/>
       <c r="C170" s="28" t="s">
         <v>170</v>
       </c>
@@ -24336,7 +24624,7 @@
       <c r="A171" s="26">
         <v>25</v>
       </c>
-      <c r="B171" s="72"/>
+      <c r="B171" s="74"/>
       <c r="C171" s="28" t="s">
         <v>171</v>
       </c>
@@ -24356,7 +24644,7 @@
       <c r="A172" s="26">
         <v>26</v>
       </c>
-      <c r="B172" s="72"/>
+      <c r="B172" s="74"/>
       <c r="C172" s="28" t="s">
         <v>40</v>
       </c>
@@ -24376,7 +24664,7 @@
       <c r="A173" s="26">
         <v>27</v>
       </c>
-      <c r="B173" s="71" t="s">
+      <c r="B173" s="75" t="s">
         <v>7</v>
       </c>
       <c r="C173" s="28" t="s">
@@ -24400,7 +24688,7 @@
       <c r="A174" s="26">
         <v>28</v>
       </c>
-      <c r="B174" s="72"/>
+      <c r="B174" s="74"/>
       <c r="C174" s="27" t="s">
         <v>175</v>
       </c>
@@ -24422,7 +24710,7 @@
       <c r="A175" s="26">
         <v>29</v>
       </c>
-      <c r="B175" s="72"/>
+      <c r="B175" s="74"/>
       <c r="C175" s="28" t="s">
         <v>178</v>
       </c>
@@ -24444,7 +24732,7 @@
       <c r="A176" s="26">
         <v>30</v>
       </c>
-      <c r="B176" s="76" t="s">
+      <c r="B176" s="84" t="s">
         <v>8</v>
       </c>
       <c r="C176" s="28" t="s">
@@ -24470,7 +24758,7 @@
       <c r="A177" s="31">
         <v>31</v>
       </c>
-      <c r="B177" s="77"/>
+      <c r="B177" s="85"/>
       <c r="C177" s="32" t="s">
         <v>183</v>
       </c>
@@ -24494,7 +24782,7 @@
       <c r="A178" s="23">
         <v>32</v>
       </c>
-      <c r="B178" s="80" t="s">
+      <c r="B178" s="86" t="s">
         <v>185</v>
       </c>
       <c r="C178" s="33" t="s">
@@ -24518,7 +24806,7 @@
       <c r="A179" s="26">
         <v>33</v>
       </c>
-      <c r="B179" s="81"/>
+      <c r="B179" s="87"/>
       <c r="C179" s="27" t="s">
         <v>189</v>
       </c>
@@ -24540,7 +24828,7 @@
       <c r="A180" s="26">
         <v>34</v>
       </c>
-      <c r="B180" s="82"/>
+      <c r="B180" s="88"/>
       <c r="C180" s="34" t="s">
         <v>192</v>
       </c>
@@ -24562,7 +24850,7 @@
       <c r="A181" s="31">
         <v>35</v>
       </c>
-      <c r="B181" s="82"/>
+      <c r="B181" s="88"/>
       <c r="C181" s="34" t="s">
         <v>193</v>
       </c>
@@ -24584,17 +24872,17 @@
       <c r="A182" s="31">
         <v>36</v>
       </c>
-      <c r="B182" s="82"/>
+      <c r="B182" s="88"/>
       <c r="C182" s="34" t="s">
         <v>196</v>
       </c>
-      <c r="D182" s="42" t="s">
+      <c r="D182" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E182" s="42" t="s">
+      <c r="E182" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F182" s="42"/>
+      <c r="F182" s="32"/>
       <c r="G182" s="34" t="s">
         <v>254</v>
       </c>
@@ -24604,15 +24892,15 @@
       <c r="A183" s="31">
         <v>37</v>
       </c>
-      <c r="B183" s="82"/>
+      <c r="B183" s="88"/>
       <c r="C183" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="D183" s="42" t="s">
+      <c r="D183" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E183" s="42"/>
-      <c r="F183" s="42" t="s">
+      <c r="E183" s="32"/>
+      <c r="F183" s="32" t="s">
         <v>249</v>
       </c>
       <c r="G183" s="34" t="s">
@@ -24653,7 +24941,7 @@
       </c>
     </row>
     <row r="186" spans="1:8">
-      <c r="B186" s="37" t="s">
+      <c r="B186" s="6" t="s">
         <v>199</v>
       </c>
     </row>
@@ -24674,280 +24962,280 @@
       <c r="A198" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="B198" s="38" t="s">
+      <c r="B198" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="C198" s="84" t="s">
+      <c r="C198" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="D198" s="84"/>
-      <c r="E198" s="84"/>
-      <c r="F198" s="39" t="s">
+      <c r="D198" s="89"/>
+      <c r="E198" s="89"/>
+      <c r="F198" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="G198" s="40" t="s">
+      <c r="G198" s="38" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="199" spans="1:7">
-      <c r="A199" s="85" t="s">
+      <c r="A199" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="B199" s="72" t="s">
+      <c r="B199" s="74" t="s">
         <v>207</v>
       </c>
-      <c r="C199" s="87" t="s">
+      <c r="C199" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="D199" s="88"/>
-      <c r="E199" s="88"/>
+      <c r="D199" s="92"/>
+      <c r="E199" s="92"/>
       <c r="F199" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="G199" s="41" t="s">
+      <c r="G199" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="85"/>
-      <c r="B200" s="86"/>
-      <c r="C200" s="89" t="s">
+      <c r="A200" s="72"/>
+      <c r="B200" s="90"/>
+      <c r="C200" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="D200" s="90"/>
-      <c r="E200" s="90"/>
+      <c r="D200" s="94"/>
+      <c r="E200" s="94"/>
       <c r="F200" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="G200" s="43" t="s">
+      <c r="G200" s="40" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="85"/>
-      <c r="B201" s="72" t="s">
+      <c r="A201" s="72"/>
+      <c r="B201" s="74" t="s">
         <v>210</v>
       </c>
-      <c r="C201" s="91" t="s">
+      <c r="C201" s="95" t="s">
         <v>211</v>
       </c>
-      <c r="D201" s="91"/>
-      <c r="E201" s="91"/>
+      <c r="D201" s="95"/>
+      <c r="E201" s="95"/>
       <c r="F201" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="G201" s="41" t="s">
+      <c r="G201" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="85"/>
-      <c r="B202" s="72"/>
-      <c r="C202" s="89" t="s">
+      <c r="A202" s="72"/>
+      <c r="B202" s="74"/>
+      <c r="C202" s="93" t="s">
         <v>211</v>
       </c>
-      <c r="D202" s="89"/>
-      <c r="E202" s="89"/>
+      <c r="D202" s="93"/>
+      <c r="E202" s="93"/>
       <c r="F202" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="G202" s="41" t="s">
+      <c r="G202" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="85"/>
-      <c r="B203" s="86" t="s">
+      <c r="A203" s="72"/>
+      <c r="B203" s="90" t="s">
         <v>212</v>
       </c>
-      <c r="C203" s="92" t="s">
+      <c r="C203" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="D203" s="93"/>
-      <c r="E203" s="94"/>
+      <c r="D203" s="97"/>
+      <c r="E203" s="98"/>
       <c r="F203" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="G203" s="41" t="s">
+      <c r="G203" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="85"/>
-      <c r="B204" s="78"/>
-      <c r="C204" s="92" t="s">
+      <c r="A204" s="72"/>
+      <c r="B204" s="79"/>
+      <c r="C204" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="D204" s="93"/>
-      <c r="E204" s="94"/>
+      <c r="D204" s="97"/>
+      <c r="E204" s="98"/>
       <c r="F204" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="G204" s="41" t="s">
+      <c r="G204" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="85"/>
-      <c r="B205" s="72" t="s">
+      <c r="A205" s="72"/>
+      <c r="B205" s="74" t="s">
         <v>213</v>
       </c>
-      <c r="C205" s="91" t="s">
+      <c r="C205" s="95" t="s">
         <v>214</v>
       </c>
-      <c r="D205" s="91"/>
-      <c r="E205" s="91"/>
+      <c r="D205" s="95"/>
+      <c r="E205" s="95"/>
       <c r="F205" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="G205" s="41" t="s">
+      <c r="G205" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="85"/>
-      <c r="B206" s="72"/>
-      <c r="C206" s="91" t="s">
+      <c r="A206" s="72"/>
+      <c r="B206" s="74"/>
+      <c r="C206" s="95" t="s">
         <v>214</v>
       </c>
-      <c r="D206" s="91"/>
-      <c r="E206" s="91"/>
+      <c r="D206" s="95"/>
+      <c r="E206" s="95"/>
       <c r="F206" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="G206" s="41" t="s">
+      <c r="G206" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="85" t="s">
+      <c r="A207" s="72" t="s">
         <v>215</v>
       </c>
-      <c r="B207" s="72" t="s">
+      <c r="B207" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="C207" s="71" t="s">
+      <c r="C207" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="D207" s="72"/>
-      <c r="E207" s="72"/>
+      <c r="D207" s="74"/>
+      <c r="E207" s="74"/>
       <c r="F207" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="G207" s="41" t="s">
+      <c r="G207" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="85"/>
-      <c r="B208" s="72"/>
-      <c r="C208" s="72" t="s">
+      <c r="A208" s="72"/>
+      <c r="B208" s="74"/>
+      <c r="C208" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="D208" s="72"/>
-      <c r="E208" s="72"/>
+      <c r="D208" s="74"/>
+      <c r="E208" s="74"/>
       <c r="F208" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="G208" s="41" t="s">
+      <c r="G208" s="39" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="85"/>
-      <c r="B209" s="72" t="s">
+      <c r="A209" s="72"/>
+      <c r="B209" s="74" t="s">
         <v>218</v>
       </c>
-      <c r="C209" s="72" t="s">
+      <c r="C209" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="D209" s="72"/>
-      <c r="E209" s="72"/>
+      <c r="D209" s="74"/>
+      <c r="E209" s="74"/>
       <c r="F209" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="G209" s="41" t="s">
+      <c r="G209" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="85"/>
-      <c r="B210" s="72"/>
-      <c r="C210" s="72" t="s">
+      <c r="A210" s="72"/>
+      <c r="B210" s="74"/>
+      <c r="C210" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="D210" s="72"/>
-      <c r="E210" s="72"/>
+      <c r="D210" s="74"/>
+      <c r="E210" s="74"/>
       <c r="F210" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="G210" s="41" t="s">
+      <c r="G210" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="85" t="s">
+      <c r="A211" s="72" t="s">
         <v>219</v>
       </c>
-      <c r="B211" s="72" t="s">
+      <c r="B211" s="74" t="s">
         <v>220</v>
       </c>
-      <c r="C211" s="71" t="s">
+      <c r="C211" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="D211" s="72"/>
-      <c r="E211" s="72"/>
+      <c r="D211" s="74"/>
+      <c r="E211" s="74"/>
       <c r="F211" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="G211" s="41" t="s">
+      <c r="G211" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="85"/>
-      <c r="B212" s="72"/>
-      <c r="C212" s="72" t="s">
+      <c r="A212" s="72"/>
+      <c r="B212" s="74"/>
+      <c r="C212" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="D212" s="72"/>
-      <c r="E212" s="72"/>
+      <c r="D212" s="74"/>
+      <c r="E212" s="74"/>
       <c r="F212" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="G212" s="41" t="s">
+      <c r="G212" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="85"/>
-      <c r="B213" s="72" t="s">
+      <c r="A213" s="72"/>
+      <c r="B213" s="74" t="s">
         <v>221</v>
       </c>
-      <c r="C213" s="71" t="s">
+      <c r="C213" s="75" t="s">
         <v>222</v>
       </c>
-      <c r="D213" s="72"/>
-      <c r="E213" s="72"/>
+      <c r="D213" s="74"/>
+      <c r="E213" s="74"/>
       <c r="F213" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="G213" s="41" t="s">
+      <c r="G213" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="214" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A214" s="96"/>
-      <c r="B214" s="97"/>
-      <c r="C214" s="97" t="s">
+      <c r="A214" s="73"/>
+      <c r="B214" s="76"/>
+      <c r="C214" s="76" t="s">
         <v>223</v>
       </c>
-      <c r="D214" s="97"/>
-      <c r="E214" s="97"/>
+      <c r="D214" s="76"/>
+      <c r="E214" s="76"/>
       <c r="F214" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="G214" s="44" t="s">
+      <c r="G214" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -24955,60 +25243,43 @@
       <c r="A215" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C215" s="37"/>
-      <c r="D215" s="37"/>
-      <c r="E215" s="37"/>
-      <c r="F215" s="37"/>
-    </row>
-    <row r="216" spans="1:7">
-      <c r="C216" s="37"/>
-      <c r="D216" s="37"/>
-      <c r="E216" s="37"/>
-    </row>
-    <row r="217" spans="1:7">
-      <c r="C217" s="37"/>
-      <c r="D217" s="37"/>
-      <c r="E217" s="37"/>
     </row>
     <row r="218" spans="1:7" ht="15.75" thickBot="1">
       <c r="A218" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C218" s="37"/>
-      <c r="D218" s="37"/>
-      <c r="E218" s="37"/>
     </row>
     <row r="219" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A219" s="45" t="s">
+      <c r="A219" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="B219" s="98" t="s">
+      <c r="B219" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="C219" s="98"/>
-      <c r="D219" s="98"/>
-      <c r="E219" s="98"/>
-      <c r="F219" s="46" t="s">
+      <c r="C219" s="77"/>
+      <c r="D219" s="77"/>
+      <c r="E219" s="77"/>
+      <c r="F219" s="43" t="s">
         <v>227</v>
       </c>
-      <c r="G219" s="47" t="s">
+      <c r="G219" s="44" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="93" customHeight="1">
-      <c r="A220" s="48" t="s">
+      <c r="A220" s="45" t="s">
         <v>229</v>
       </c>
-      <c r="B220" s="99" t="s">
+      <c r="B220" s="78" t="s">
         <v>230</v>
       </c>
-      <c r="C220" s="78"/>
-      <c r="D220" s="78"/>
-      <c r="E220" s="78"/>
-      <c r="F220" s="49" t="s">
+      <c r="C220" s="79"/>
+      <c r="D220" s="79"/>
+      <c r="E220" s="79"/>
+      <c r="F220" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="G220" s="50" t="s">
+      <c r="G220" s="47" t="s">
         <v>62</v>
       </c>
     </row>
@@ -25016,12 +25287,12 @@
       <c r="A221" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="B221" s="100" t="s">
+      <c r="B221" s="80" t="s">
         <v>232</v>
       </c>
-      <c r="C221" s="101"/>
-      <c r="D221" s="101"/>
-      <c r="E221" s="102"/>
+      <c r="C221" s="81"/>
+      <c r="D221" s="81"/>
+      <c r="E221" s="82"/>
       <c r="F221" s="15" t="s">
         <v>62</v>
       </c>
@@ -25033,12 +25304,12 @@
       <c r="A222" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B222" s="100" t="s">
+      <c r="B222" s="80" t="s">
         <v>233</v>
       </c>
-      <c r="C222" s="101"/>
-      <c r="D222" s="101"/>
-      <c r="E222" s="102"/>
+      <c r="C222" s="81"/>
+      <c r="D222" s="81"/>
+      <c r="E222" s="82"/>
       <c r="F222" s="18" t="s">
         <v>62</v>
       </c>
@@ -25053,9 +25324,9 @@
       <c r="B223" s="83" t="s">
         <v>235</v>
       </c>
-      <c r="C223" s="97"/>
-      <c r="D223" s="97"/>
-      <c r="E223" s="97"/>
+      <c r="C223" s="76"/>
+      <c r="D223" s="76"/>
+      <c r="E223" s="76"/>
       <c r="F223" s="21" t="s">
         <v>62</v>
       </c>
@@ -25064,7 +25335,7 @@
       </c>
     </row>
     <row r="224" spans="1:7">
-      <c r="C224" s="51"/>
+      <c r="C224" s="48"/>
     </row>
     <row r="226" spans="1:7" ht="15.75" thickBot="1">
       <c r="A226" s="6" t="s">
@@ -25075,302 +25346,279 @@
       <c r="A227" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="B227" s="38" t="s">
+      <c r="B227" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C227" s="52" t="s">
+      <c r="C227" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="D227" s="53" t="s">
+      <c r="D227" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="E227" s="53"/>
-      <c r="F227" s="54"/>
-      <c r="G227" s="40" t="s">
+      <c r="E227" s="50"/>
+      <c r="F227" s="10"/>
+      <c r="G227" s="38" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="228" spans="1:7">
-      <c r="A228" s="55">
+      <c r="A228" s="51">
         <v>42682</v>
       </c>
-      <c r="B228" s="56">
+      <c r="B228" s="52">
         <v>1.04</v>
       </c>
       <c r="C228" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D228" s="95" t="s">
+      <c r="D228" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="E228" s="95"/>
-      <c r="F228" s="95"/>
-      <c r="G228" s="57"/>
+      <c r="E228" s="71"/>
+      <c r="F228" s="71"/>
+      <c r="G228" s="25"/>
     </row>
     <row r="229" spans="1:7">
-      <c r="A229" s="58">
+      <c r="A229" s="53">
         <v>42692</v>
       </c>
-      <c r="B229" s="59">
+      <c r="B229" s="54">
         <v>1.05</v>
       </c>
       <c r="C229" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D229" s="107" t="s">
+      <c r="D229" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="E229" s="107"/>
-      <c r="F229" s="107"/>
-      <c r="G229" s="41"/>
+      <c r="E229" s="70"/>
+      <c r="F229" s="70"/>
+      <c r="G229" s="39"/>
     </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="58">
+      <c r="A230" s="53">
         <v>42955</v>
       </c>
-      <c r="B230" s="59">
+      <c r="B230" s="54">
         <v>1.06</v>
       </c>
       <c r="C230" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D230" s="107" t="s">
+      <c r="D230" s="70" t="s">
         <v>239</v>
       </c>
-      <c r="E230" s="107"/>
-      <c r="F230" s="107"/>
-      <c r="G230" s="41"/>
+      <c r="E230" s="70"/>
+      <c r="F230" s="70"/>
+      <c r="G230" s="39"/>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="58">
+      <c r="A231" s="53">
         <v>42991</v>
       </c>
-      <c r="B231" s="59">
+      <c r="B231" s="54">
         <v>1.07</v>
       </c>
       <c r="C231" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D231" s="107" t="s">
+      <c r="D231" s="70" t="s">
         <v>240</v>
       </c>
-      <c r="E231" s="107"/>
-      <c r="F231" s="107"/>
-      <c r="G231" s="41"/>
+      <c r="E231" s="70"/>
+      <c r="F231" s="70"/>
+      <c r="G231" s="39"/>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="58">
+      <c r="A232" s="53">
         <v>43026</v>
       </c>
-      <c r="B232" s="59">
+      <c r="B232" s="54">
         <v>1.08</v>
       </c>
       <c r="C232" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D232" s="107" t="s">
+      <c r="D232" s="70" t="s">
         <v>241</v>
       </c>
-      <c r="E232" s="107"/>
-      <c r="F232" s="107"/>
-      <c r="G232" s="41"/>
+      <c r="E232" s="70"/>
+      <c r="F232" s="70"/>
+      <c r="G232" s="39"/>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="58">
+      <c r="A233" s="53">
         <v>43069</v>
       </c>
-      <c r="B233" s="59">
+      <c r="B233" s="54">
         <v>1.0900000000000001</v>
       </c>
       <c r="C233" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D233" s="107" t="s">
+      <c r="D233" s="70" t="s">
         <v>242</v>
       </c>
-      <c r="E233" s="107"/>
-      <c r="F233" s="107"/>
-      <c r="G233" s="41"/>
+      <c r="E233" s="70"/>
+      <c r="F233" s="70"/>
+      <c r="G233" s="39"/>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="60">
+      <c r="A234" s="55">
         <v>43248</v>
       </c>
-      <c r="B234" s="61">
+      <c r="B234" s="56">
         <v>1.1000000000000001</v>
       </c>
       <c r="C234" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D234" s="103" t="s">
+      <c r="D234" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="E234" s="104"/>
-      <c r="F234" s="105"/>
-      <c r="G234" s="43"/>
+      <c r="E234" s="67"/>
+      <c r="F234" s="68"/>
+      <c r="G234" s="40"/>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="60">
+      <c r="A235" s="55">
         <v>43339</v>
       </c>
-      <c r="B235" s="61">
+      <c r="B235" s="56">
         <v>1.1100000000000001</v>
       </c>
       <c r="C235" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D235" s="103" t="s">
+      <c r="D235" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="E235" s="104"/>
-      <c r="F235" s="105"/>
-      <c r="G235" s="43"/>
+      <c r="E235" s="67"/>
+      <c r="F235" s="68"/>
+      <c r="G235" s="40"/>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="60">
+      <c r="A236" s="55">
         <v>43542</v>
       </c>
-      <c r="B236" s="61">
+      <c r="B236" s="56">
         <v>1.1200000000000001</v>
       </c>
       <c r="C236" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D236" s="103" t="s">
+      <c r="D236" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="E236" s="104"/>
-      <c r="F236" s="105"/>
-      <c r="G236" s="43"/>
+      <c r="E236" s="67"/>
+      <c r="F236" s="68"/>
+      <c r="G236" s="40"/>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="60">
+      <c r="A237" s="55">
         <v>43599</v>
       </c>
-      <c r="B237" s="61">
+      <c r="B237" s="56">
         <v>1.1299999999999999</v>
       </c>
       <c r="C237" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D237" s="62" t="s">
+      <c r="D237" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="E237" s="63"/>
-      <c r="F237" s="64"/>
-      <c r="G237" s="43"/>
+      <c r="E237" s="58"/>
+      <c r="F237" s="59"/>
+      <c r="G237" s="40"/>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="60">
+      <c r="A238" s="55">
         <v>43643</v>
       </c>
-      <c r="B238" s="61">
+      <c r="B238" s="56">
         <v>1.1399999999999999</v>
       </c>
       <c r="C238" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D238" s="62" t="s">
+      <c r="D238" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="E238" s="63"/>
-      <c r="F238" s="64"/>
-      <c r="G238" s="43"/>
+      <c r="E238" s="58"/>
+      <c r="F238" s="59"/>
+      <c r="G238" s="40"/>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="60">
+      <c r="A239" s="55">
         <v>43894</v>
       </c>
-      <c r="B239" s="61">
+      <c r="B239" s="56">
         <v>1.1499999999999999</v>
       </c>
       <c r="C239" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D239" s="62" t="s">
+      <c r="D239" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="E239" s="63"/>
-      <c r="F239" s="64"/>
-      <c r="G239" s="43"/>
+      <c r="E239" s="58"/>
+      <c r="F239" s="59"/>
+      <c r="G239" s="40"/>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="60">
+      <c r="A240" s="55">
         <v>44017</v>
       </c>
-      <c r="B240" s="61">
+      <c r="B240" s="56">
         <v>1.1599999999999999</v>
       </c>
-      <c r="C240" s="42" t="s">
+      <c r="C240" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D240" s="62" t="s">
+      <c r="D240" s="57" t="s">
         <v>243</v>
       </c>
-      <c r="E240" s="63"/>
-      <c r="F240" s="64"/>
-      <c r="G240" s="43"/>
+      <c r="E240" s="58"/>
+      <c r="F240" s="59"/>
+      <c r="G240" s="40"/>
     </row>
     <row r="241" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A241" s="65">
+      <c r="A241" s="60">
         <v>44118</v>
       </c>
-      <c r="B241" s="66">
+      <c r="B241" s="61">
         <v>1.17</v>
       </c>
       <c r="C241" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="D241" s="106" t="s">
+      <c r="D241" s="69" t="s">
         <v>255</v>
       </c>
-      <c r="E241" s="106"/>
-      <c r="F241" s="106"/>
-      <c r="G241" s="44"/>
+      <c r="E241" s="69"/>
+      <c r="F241" s="69"/>
+      <c r="G241" s="41"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ap+vydlQsTivses2kTOZJOfe+E+ofk18ovQVkbwX/cy/2QzQqNYlkd6ZRwhTqYv60tXLJj9O4rjHfeOPlaqbDA==" saltValue="NIz07f4XZ+x9XJy8gC1img==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait"/>
-    </customSheetView>
     <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" scale="115" topLeftCell="A172">
       <selection activeCell="C180" sqref="C180"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D241:F241"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D228:F228"/>
-    <mergeCell ref="A211:A214"/>
-    <mergeCell ref="B211:B212"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="B213:B214"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="B219:E219"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="A207:A210"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="C207:E207"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="B209:B210"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="B173:B175"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B147:B159"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="B162:B164"/>
+    <mergeCell ref="B165:B172"/>
     <mergeCell ref="B176:B177"/>
     <mergeCell ref="B178:B184"/>
     <mergeCell ref="C198:E198"/>
@@ -25387,12 +25635,35 @@
     <mergeCell ref="B205:B206"/>
     <mergeCell ref="C205:E205"/>
     <mergeCell ref="C206:E206"/>
-    <mergeCell ref="B173:B175"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B147:B159"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="B165:B172"/>
+    <mergeCell ref="A207:A210"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="B209:B210"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="D228:F228"/>
+    <mergeCell ref="A211:A214"/>
+    <mergeCell ref="B211:B212"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="B213:B214"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="B219:E219"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D241:F241"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -25401,7 +25672,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -25415,18 +25686,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i499--EIT2 suite files update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_04_jedi.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_04_jedi.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzhou2\Desktop\00_TMP_Client\new\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{5DF25FC7-3CE5-460C-B8E1-871B1CE9E034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{5DFB4C1B-5A2C-4BAF-972B-F1CEE14537C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="BBPw5sjxCCUVqKqDFh1VvlGl+6jBsyEv58ubpDIjFduKT4EttifNtZLgNn2j4jGi/bvDsFNRyO0+XWiClC3JHw==" workbookSaltValue="FQsz7bLsuDdqgfH6Nya7QA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,15 @@
     <definedName name="Z_16B2C8B3_13FA_43FB_96C1_3763C72619A6_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
     <definedName name="Z_179F0E1F_F6F7_410E_B883_54B8A90BA550_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
     <definedName name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
+    <definedName name="Z_FFCBA651_8693_4F31_A4A9_0AA919B68C0C_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
   </definedNames>
-  <calcPr calcId="122211" calcOnSave="0"/>
+  <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jerry (Chenghan) Zhou - Personal View" guid="{FFCBA651-8693-4F31-A4A9-0AA919B68C0C}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1048" activeSheetId="2"/>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Cherry (Ying) Xu - Personal View" guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -970,9 +972,6 @@
     <t>00_primitive/01_clock/11_PCLKDIVSP</t>
   </si>
   <si>
-    <t>00_primitive/01_clock/12_PLL</t>
-  </si>
-  <si>
     <t>cmd = --run-ipgen</t>
   </si>
   <si>
@@ -1238,6 +1237,9 @@
   </si>
   <si>
     <t>Jason.Wang</t>
+  </si>
+  <si>
+    <t>00_primitive/01_clock/12_PLLA</t>
   </si>
 </sst>
 </file>
@@ -2525,64 +2527,31 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2594,7 +2563,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2614,17 +2589,44 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -5163,7 +5165,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0AF23792-2803-4DFD-B32E-BC59B929B60B}" diskRevisions="1" revisionId="1558" version="31">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{71EBCED0-4CC4-4056-9FC2-8FD06E1FE8BE}" diskRevisions="1" revisionId="1560" version="32">
   <header guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" dateTime="2020-10-15T13:42:26" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5412,6 +5414,14 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{71EBCED0-4CC4-4056-9FC2-8FD06E1FE8BE}" dateTime="2024-05-29T15:32:12" maxSheetId="5" userName="Jerry (Chenghan) Zhou" r:id="rId32" minRId="1559">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -13042,6 +13052,27 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog32.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1559" sId="2">
+    <oc r="E33" t="inlineStr">
+      <is>
+        <t>00_primitive/01_clock/12_PLL</t>
+      </is>
+    </oc>
+    <nc r="E33" t="inlineStr">
+      <is>
+        <t>00_primitive/01_clock/12_PLLA</t>
+      </is>
+    </nc>
+  </rcc>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_FFCBA651_8693_4F31_A4A9_0AA919B68C0C_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+  </rdn>
+  <rcv guid="{FFCBA651-8693-4F31-A4A9-0AA919B68C0C}" action="add"/>
 </revisions>
 </file>
 
@@ -20787,7 +20818,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
   <userInfo guid="{EF406D44-8062-40DE-A000-69E56EC874B5}" name="Cherry (Ying) Xu" id="-707422276" dateTime="2020-11-23T15:52:35"/>
 </users>
@@ -21082,7 +21113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -21098,7 +21129,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -21114,7 +21145,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -21148,7 +21179,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -21207,7 +21238,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -21267,13 +21298,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}">
-      <selection activeCell="C37" sqref="C37"/>
+    <customSheetView guid="{FFCBA651-8693-4F31-A4A9-0AA919B68C0C}">
+      <selection activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B27" sqref="B27"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -21282,15 +21313,20 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B27" sqref="B27"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+    </customSheetView>
+    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}">
+      <selection activeCell="C37" sqref="C37"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -21298,12 +21334,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD114"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B114" sqref="B114"/>
+      <selection pane="bottomRight" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -21471,10 +21507,10 @@
         <v>270</v>
       </c>
       <c r="S3" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD3" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -21485,10 +21521,10 @@
         <v>271</v>
       </c>
       <c r="S4" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD4" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -21499,7 +21535,7 @@
         <v>272</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD5" s="2" t="s">
         <v>261</v>
@@ -21513,10 +21549,10 @@
         <v>273</v>
       </c>
       <c r="S6" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD6" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -21527,10 +21563,10 @@
         <v>274</v>
       </c>
       <c r="S7" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD7" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD7" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -21541,10 +21577,10 @@
         <v>275</v>
       </c>
       <c r="S8" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD8" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -21555,10 +21591,10 @@
         <v>276</v>
       </c>
       <c r="S9" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD9" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD9" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -21569,10 +21605,10 @@
         <v>277</v>
       </c>
       <c r="S10" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD10" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD10" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -21583,10 +21619,10 @@
         <v>278</v>
       </c>
       <c r="S11" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD11" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD11" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -21597,10 +21633,10 @@
         <v>279</v>
       </c>
       <c r="S12" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD12" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD12" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -21611,10 +21647,10 @@
         <v>280</v>
       </c>
       <c r="S13" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD13" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD13" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:30">
@@ -21625,10 +21661,10 @@
         <v>281</v>
       </c>
       <c r="S14" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD14" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD14" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="15" spans="1:30">
@@ -21639,10 +21675,10 @@
         <v>282</v>
       </c>
       <c r="S15" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD15" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD15" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -21653,10 +21689,10 @@
         <v>283</v>
       </c>
       <c r="S16" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD16" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD16" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="17" spans="1:30">
@@ -21667,10 +21703,10 @@
         <v>284</v>
       </c>
       <c r="S17" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD17" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD17" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:30">
@@ -21681,10 +21717,10 @@
         <v>285</v>
       </c>
       <c r="S18" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD18" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD18" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="19" spans="1:30">
@@ -21695,10 +21731,10 @@
         <v>286</v>
       </c>
       <c r="S19" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD19" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD19" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="20" spans="1:30">
@@ -21709,10 +21745,10 @@
         <v>287</v>
       </c>
       <c r="S20" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD20" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD20" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="21" spans="1:30">
@@ -21723,10 +21759,10 @@
         <v>288</v>
       </c>
       <c r="S21" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD21" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD21" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="22" spans="1:30">
@@ -21737,7 +21773,7 @@
         <v>289</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD22" s="2" t="s">
         <v>261</v>
@@ -21751,10 +21787,10 @@
         <v>290</v>
       </c>
       <c r="S23" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD23" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD23" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="24" spans="1:30">
@@ -21765,7 +21801,7 @@
         <v>291</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD24" s="2" t="s">
         <v>261</v>
@@ -21779,7 +21815,7 @@
         <v>292</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD25" s="2" t="s">
         <v>261</v>
@@ -21793,7 +21829,7 @@
         <v>293</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD26" s="2" t="s">
         <v>261</v>
@@ -21807,7 +21843,7 @@
         <v>294</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD27" s="2" t="s">
         <v>261</v>
@@ -21821,7 +21857,7 @@
         <v>295</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD28" s="2" t="s">
         <v>261</v>
@@ -21835,10 +21871,10 @@
         <v>296</v>
       </c>
       <c r="S29" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD29" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD29" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="30" spans="1:30">
@@ -21849,7 +21885,7 @@
         <v>297</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD30" s="2" t="s">
         <v>261</v>
@@ -21863,10 +21899,10 @@
         <v>298</v>
       </c>
       <c r="S31" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD31" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD31" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="32" spans="1:30">
@@ -21877,10 +21913,10 @@
         <v>299</v>
       </c>
       <c r="S32" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD32" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD32" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="33" spans="1:30">
@@ -21888,16 +21924,16 @@
         <v>31</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="O33" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="O33" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="S33" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD33" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD33" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="34" spans="1:30">
@@ -21905,13 +21941,13 @@
         <v>32</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD34" s="2" t="s">
         <v>261</v>
@@ -21922,13 +21958,13 @@
         <v>33</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="S35" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD35" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD35" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="36" spans="1:30">
@@ -21936,13 +21972,13 @@
         <v>34</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="S36" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD36" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD36" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="37" spans="1:30">
@@ -21950,13 +21986,13 @@
         <v>35</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="S37" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD37" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD37" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="38" spans="1:30">
@@ -21964,13 +22000,13 @@
         <v>36</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="S38" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD38" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD38" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="39" spans="1:30">
@@ -21978,10 +22014,10 @@
         <v>37</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD39" s="2" t="s">
         <v>261</v>
@@ -21992,13 +22028,13 @@
         <v>38</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="S40" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD40" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD40" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="41" spans="1:30">
@@ -22006,13 +22042,13 @@
         <v>39</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="S41" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD41" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD41" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="42" spans="1:30">
@@ -22020,13 +22056,13 @@
         <v>40</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S42" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD42" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD42" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="43" spans="1:30">
@@ -22034,13 +22070,13 @@
         <v>41</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="S43" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD43" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD43" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="44" spans="1:30">
@@ -22048,13 +22084,13 @@
         <v>42</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="S44" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD44" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD44" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="45" spans="1:30">
@@ -22062,13 +22098,13 @@
         <v>43</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="S45" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD45" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD45" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="46" spans="1:30">
@@ -22076,13 +22112,13 @@
         <v>44</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="S46" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD46" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD46" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="47" spans="1:30">
@@ -22090,13 +22126,13 @@
         <v>45</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S47" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD47" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD47" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="48" spans="1:30">
@@ -22104,13 +22140,13 @@
         <v>46</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S48" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD48" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD48" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="49" spans="1:30">
@@ -22118,13 +22154,13 @@
         <v>47</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S49" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD49" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD49" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="50" spans="1:30">
@@ -22132,13 +22168,13 @@
         <v>48</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S50" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD50" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD50" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="51" spans="1:30">
@@ -22146,13 +22182,13 @@
         <v>49</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="S51" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD51" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD51" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="52" spans="1:30">
@@ -22160,13 +22196,13 @@
         <v>50</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="S52" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD52" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD52" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="53" spans="1:30">
@@ -22174,13 +22210,13 @@
         <v>51</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="S53" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD53" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD53" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="54" spans="1:30">
@@ -22188,13 +22224,13 @@
         <v>52</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="S54" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD54" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD54" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="55" spans="1:30">
@@ -22202,13 +22238,13 @@
         <v>53</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="S55" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD55" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD55" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="56" spans="1:30">
@@ -22216,13 +22252,13 @@
         <v>54</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="S56" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD56" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD56" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="57" spans="1:30">
@@ -22230,13 +22266,13 @@
         <v>55</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="S57" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD57" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD57" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="58" spans="1:30">
@@ -22244,13 +22280,13 @@
         <v>56</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="S58" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD58" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD58" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="59" spans="1:30">
@@ -22258,13 +22294,13 @@
         <v>57</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S59" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD59" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD59" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="60" spans="1:30">
@@ -22272,13 +22308,13 @@
         <v>58</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="S60" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD60" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD60" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="61" spans="1:30">
@@ -22286,13 +22322,13 @@
         <v>59</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="S61" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD61" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD61" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="62" spans="1:30">
@@ -22300,13 +22336,13 @@
         <v>60</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="S62" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD62" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD62" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="63" spans="1:30">
@@ -22314,13 +22350,13 @@
         <v>61</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S63" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD63" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD63" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="64" spans="1:30">
@@ -22328,13 +22364,13 @@
         <v>62</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="S64" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD64" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD64" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="65" spans="1:30">
@@ -22342,13 +22378,13 @@
         <v>63</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="S65" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD65" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD65" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="66" spans="1:30">
@@ -22356,13 +22392,13 @@
         <v>64</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="S66" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD66" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD66" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="67" spans="1:30">
@@ -22370,13 +22406,13 @@
         <v>65</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="S67" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD67" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD67" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="68" spans="1:30">
@@ -22384,13 +22420,13 @@
         <v>66</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="S68" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD68" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD68" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="69" spans="1:30">
@@ -22398,13 +22434,13 @@
         <v>67</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S69" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD69" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD69" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="70" spans="1:30">
@@ -22412,13 +22448,13 @@
         <v>68</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="S70" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD70" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD70" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="71" spans="1:30">
@@ -22426,10 +22462,10 @@
         <v>69</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="S71" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD71" s="2" t="s">
         <v>261</v>
@@ -22440,13 +22476,13 @@
         <v>70</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="S72" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD72" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD72" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="73" spans="1:30">
@@ -22454,13 +22490,13 @@
         <v>71</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="S73" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD73" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD73" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="74" spans="1:30">
@@ -22468,10 +22504,10 @@
         <v>72</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="S74" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD74" s="2" t="s">
         <v>261</v>
@@ -22482,13 +22518,13 @@
         <v>73</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="S75" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD75" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD75" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="76" spans="1:30">
@@ -22496,13 +22532,13 @@
         <v>74</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="S76" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD76" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD76" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="77" spans="1:30">
@@ -22510,13 +22546,13 @@
         <v>75</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="S77" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD77" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD77" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="78" spans="1:30">
@@ -22524,13 +22560,13 @@
         <v>76</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S78" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD78" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD78" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="79" spans="1:30">
@@ -22538,13 +22574,13 @@
         <v>77</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="S79" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD79" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD79" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="80" spans="1:30">
@@ -22552,13 +22588,13 @@
         <v>78</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="S80" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD80" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD80" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="81" spans="1:30">
@@ -22566,13 +22602,13 @@
         <v>79</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="S81" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD81" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD81" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="82" spans="1:30">
@@ -22580,10 +22616,10 @@
         <v>80</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="S82" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD82" s="2" t="s">
         <v>261</v>
@@ -22594,13 +22630,13 @@
         <v>81</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="S83" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD83" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD83" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="84" spans="1:30">
@@ -22608,10 +22644,10 @@
         <v>82</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="S84" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD84" s="2" t="s">
         <v>261</v>
@@ -22622,13 +22658,13 @@
         <v>83</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S85" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD85" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD85" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="86" spans="1:30">
@@ -22636,13 +22672,13 @@
         <v>84</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="S86" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD86" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD86" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="87" spans="1:30">
@@ -22650,13 +22686,13 @@
         <v>85</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="S87" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD87" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD87" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="88" spans="1:30">
@@ -22664,13 +22700,13 @@
         <v>86</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S88" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD88" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD88" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="89" spans="1:30">
@@ -22678,13 +22714,13 @@
         <v>87</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="S89" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD89" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD89" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="90" spans="1:30">
@@ -22692,13 +22728,13 @@
         <v>88</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="S90" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD90" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD90" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="91" spans="1:30">
@@ -22706,13 +22742,13 @@
         <v>89</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S91" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD91" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD91" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="92" spans="1:30">
@@ -22720,13 +22756,13 @@
         <v>90</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="S92" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD92" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD92" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="93" spans="1:30">
@@ -22734,13 +22770,13 @@
         <v>91</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="S93" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD93" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD93" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="94" spans="1:30">
@@ -22748,13 +22784,13 @@
         <v>92</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="S94" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD94" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD94" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="95" spans="1:30">
@@ -22762,13 +22798,13 @@
         <v>93</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="S95" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD95" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD95" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="96" spans="1:30">
@@ -22776,13 +22812,13 @@
         <v>94</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S96" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD96" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD96" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="97" spans="1:30">
@@ -22790,13 +22826,13 @@
         <v>95</v>
       </c>
       <c r="E97" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="O97" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="O97" s="2" t="s">
-        <v>366</v>
-      </c>
       <c r="S97" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD97" s="2" t="s">
         <v>261</v>
@@ -22807,13 +22843,13 @@
         <v>96</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="S98" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD98" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD98" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="99" spans="1:30">
@@ -22821,13 +22857,13 @@
         <v>97</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="S99" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD99" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD99" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="100" spans="1:30">
@@ -22835,10 +22871,10 @@
         <v>98</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="S100" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD100" s="2" t="s">
         <v>261</v>
@@ -22849,13 +22885,13 @@
         <v>99</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S101" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD101" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD101" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="102" spans="1:30">
@@ -22863,13 +22899,13 @@
         <v>100</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="S102" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD102" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD102" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="103" spans="1:30">
@@ -22877,10 +22913,10 @@
         <v>101</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="S103" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD103" s="2" t="s">
         <v>261</v>
@@ -22891,13 +22927,13 @@
         <v>102</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="S104" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD104" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD104" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="105" spans="1:30">
@@ -22905,13 +22941,13 @@
         <v>103</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S105" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD105" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD105" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="106" spans="1:30">
@@ -22919,13 +22955,13 @@
         <v>104</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S106" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD106" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD106" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="107" spans="1:30">
@@ -22933,13 +22969,13 @@
         <v>105</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="S107" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD107" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD107" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="108" spans="1:30">
@@ -22947,10 +22983,10 @@
         <v>106</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="S108" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD108" s="2" t="s">
         <v>261</v>
@@ -22961,10 +22997,10 @@
         <v>107</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="S109" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD109" s="2" t="s">
         <v>261</v>
@@ -22975,13 +23011,13 @@
         <v>108</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="S110" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AD110" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="AD110" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="111" spans="1:30">
@@ -22989,10 +23025,10 @@
         <v>109</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="S111" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD111" s="2" t="s">
         <v>261</v>
@@ -23003,10 +23039,10 @@
         <v>110</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="S112" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD112" s="2" t="s">
         <v>261</v>
@@ -23017,10 +23053,10 @@
         <v>111</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="S113" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AD113" s="2" t="s">
         <v>261</v>
@@ -23031,10 +23067,10 @@
         <v>112</v>
       </c>
       <c r="E114" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="S114" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="S114" s="2" t="s">
-        <v>384</v>
       </c>
       <c r="AD114" s="2" t="s">
         <v>261</v>
@@ -23044,33 +23080,40 @@
   <sheetProtection algorithmName="SHA-512" hashValue="y+CBG6/YKaQ6HsaQYTqaGGAc9K7SdI4KYNN5n42I5k04yiTX0Fn8xQwrYnwNAtl9mwRmr3UcHPCrpySoPgBJNA==" saltValue="2QS/OSgjoJCpqDc5Ec8Idw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AD2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
-    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" scale="70" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="F87" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="O114" sqref="O114"/>
+    <customSheetView guid="{FFCBA651-8693-4F31-A4A9-0AA919B68C0C}" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="G35" sqref="G35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:AD2" xr:uid="{3FE11130-1CCC-45F4-B900-CA4892397AE7}"/>
+      <autoFilter ref="A2:AD2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="B116" sqref="B116"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="A2:Y2" xr:uid="{BD56282D-7EF1-48FE-80A0-25546DF1A1E1}"/>
+      <autoFilter ref="A2:AD2" xr:uid="{4E8CA741-6412-4AA7-A6A7-07605C7EE9E0}"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:Y2" xr:uid="{C6EE0AC2-197C-4D72-9F78-D0C2823AA5B9}"/>
+      <autoFilter ref="A2:Y2" xr:uid="{6201973E-0DFD-40B1-94C9-5D225DCAB44A}"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B116" sqref="B116"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-      <autoFilter ref="A2:AD2" xr:uid="{F0104AC4-58A0-4A97-A72A-A401C8821E4E}"/>
+      <autoFilter ref="A2:Y2" xr:uid="{F17B63F3-CE7C-4D39-A3F0-51625254AC45}"/>
+    </customSheetView>
+    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" scale="70" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="F87" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="O114" sqref="O114"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+      <autoFilter ref="A2:AD2" xr:uid="{28B96D42-C6B8-4ED0-A6DA-AFB027EAE486}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -23084,7 +23127,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
@@ -23206,17 +23249,17 @@
       <c r="E111" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F111" s="99" t="s">
+      <c r="F111" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="G111" s="100"/>
-      <c r="H111" s="100"/>
-      <c r="I111" s="100"/>
-      <c r="J111" s="100"/>
-      <c r="K111" s="100"/>
-      <c r="L111" s="100"/>
-      <c r="M111" s="100"/>
-      <c r="N111" s="101"/>
+      <c r="G111" s="69"/>
+      <c r="H111" s="69"/>
+      <c r="I111" s="69"/>
+      <c r="J111" s="69"/>
+      <c r="K111" s="69"/>
+      <c r="L111" s="69"/>
+      <c r="M111" s="69"/>
+      <c r="N111" s="70"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -24080,7 +24123,7 @@
       <c r="A147" s="26">
         <v>1</v>
       </c>
-      <c r="B147" s="84" t="s">
+      <c r="B147" s="71" t="s">
         <v>3</v>
       </c>
       <c r="C147" s="27" t="s">
@@ -24106,7 +24149,7 @@
       <c r="A148" s="26">
         <v>2</v>
       </c>
-      <c r="B148" s="85"/>
+      <c r="B148" s="72"/>
       <c r="C148" s="28" t="s">
         <v>130</v>
       </c>
@@ -24128,7 +24171,7 @@
       <c r="A149" s="26">
         <v>3</v>
       </c>
-      <c r="B149" s="85"/>
+      <c r="B149" s="72"/>
       <c r="C149" s="28" t="s">
         <v>9</v>
       </c>
@@ -24148,7 +24191,7 @@
       <c r="A150" s="26">
         <v>4</v>
       </c>
-      <c r="B150" s="85"/>
+      <c r="B150" s="72"/>
       <c r="C150" s="28" t="s">
         <v>132</v>
       </c>
@@ -24172,7 +24215,7 @@
       <c r="A151" s="26">
         <v>5</v>
       </c>
-      <c r="B151" s="85"/>
+      <c r="B151" s="72"/>
       <c r="C151" s="27" t="s">
         <v>134</v>
       </c>
@@ -24196,7 +24239,7 @@
       <c r="A152" s="26">
         <v>6</v>
       </c>
-      <c r="B152" s="85"/>
+      <c r="B152" s="72"/>
       <c r="C152" s="27" t="s">
         <v>138</v>
       </c>
@@ -24220,7 +24263,7 @@
       <c r="A153" s="26">
         <v>7</v>
       </c>
-      <c r="B153" s="85"/>
+      <c r="B153" s="72"/>
       <c r="C153" s="28" t="s">
         <v>141</v>
       </c>
@@ -24242,7 +24285,7 @@
       <c r="A154" s="26">
         <v>8</v>
       </c>
-      <c r="B154" s="85"/>
+      <c r="B154" s="72"/>
       <c r="C154" s="27" t="s">
         <v>142</v>
       </c>
@@ -24266,7 +24309,7 @@
       <c r="A155" s="26">
         <v>9</v>
       </c>
-      <c r="B155" s="85"/>
+      <c r="B155" s="72"/>
       <c r="C155" s="27" t="s">
         <v>143</v>
       </c>
@@ -24290,7 +24333,7 @@
       <c r="A156" s="26">
         <v>10</v>
       </c>
-      <c r="B156" s="85"/>
+      <c r="B156" s="72"/>
       <c r="C156" s="28" t="s">
         <v>144</v>
       </c>
@@ -24314,7 +24357,7 @@
       <c r="A157" s="26">
         <v>11</v>
       </c>
-      <c r="B157" s="85"/>
+      <c r="B157" s="72"/>
       <c r="C157" s="28" t="s">
         <v>145</v>
       </c>
@@ -24338,7 +24381,7 @@
       <c r="A158" s="26">
         <v>12</v>
       </c>
-      <c r="B158" s="85"/>
+      <c r="B158" s="72"/>
       <c r="C158" s="28" t="s">
         <v>147</v>
       </c>
@@ -24360,7 +24403,7 @@
       <c r="A159" s="26">
         <v>13</v>
       </c>
-      <c r="B159" s="79"/>
+      <c r="B159" s="73"/>
       <c r="C159" s="28" t="s">
         <v>55</v>
       </c>
@@ -24384,7 +24427,7 @@
       <c r="A160" s="26">
         <v>14</v>
       </c>
-      <c r="B160" s="75" t="s">
+      <c r="B160" s="66" t="s">
         <v>4</v>
       </c>
       <c r="C160" s="28" t="s">
@@ -24410,7 +24453,7 @@
       <c r="A161" s="26">
         <v>15</v>
       </c>
-      <c r="B161" s="74"/>
+      <c r="B161" s="67"/>
       <c r="C161" s="28" t="s">
         <v>155</v>
       </c>
@@ -24434,7 +24477,7 @@
       <c r="A162" s="26">
         <v>16</v>
       </c>
-      <c r="B162" s="84" t="s">
+      <c r="B162" s="71" t="s">
         <v>5</v>
       </c>
       <c r="C162" s="28" t="s">
@@ -24458,7 +24501,7 @@
       <c r="A163" s="26">
         <v>17</v>
       </c>
-      <c r="B163" s="102"/>
+      <c r="B163" s="74"/>
       <c r="C163" s="27" t="s">
         <v>159</v>
       </c>
@@ -24480,7 +24523,7 @@
       <c r="A164" s="26">
         <v>18</v>
       </c>
-      <c r="B164" s="79"/>
+      <c r="B164" s="73"/>
       <c r="C164" s="27" t="s">
         <v>161</v>
       </c>
@@ -24500,7 +24543,7 @@
       <c r="A165" s="26">
         <v>19</v>
       </c>
-      <c r="B165" s="75" t="s">
+      <c r="B165" s="66" t="s">
         <v>6</v>
       </c>
       <c r="C165" s="28" t="s">
@@ -24524,7 +24567,7 @@
       <c r="A166" s="26">
         <v>20</v>
       </c>
-      <c r="B166" s="74"/>
+      <c r="B166" s="67"/>
       <c r="C166" s="28" t="s">
         <v>166</v>
       </c>
@@ -24544,7 +24587,7 @@
       <c r="A167" s="26">
         <v>21</v>
       </c>
-      <c r="B167" s="74"/>
+      <c r="B167" s="67"/>
       <c r="C167" s="28" t="s">
         <v>167</v>
       </c>
@@ -24564,7 +24607,7 @@
       <c r="A168" s="26">
         <v>22</v>
       </c>
-      <c r="B168" s="74"/>
+      <c r="B168" s="67"/>
       <c r="C168" s="28" t="s">
         <v>168</v>
       </c>
@@ -24584,7 +24627,7 @@
       <c r="A169" s="26">
         <v>23</v>
       </c>
-      <c r="B169" s="74"/>
+      <c r="B169" s="67"/>
       <c r="C169" s="28" t="s">
         <v>169</v>
       </c>
@@ -24604,7 +24647,7 @@
       <c r="A170" s="26">
         <v>24</v>
       </c>
-      <c r="B170" s="74"/>
+      <c r="B170" s="67"/>
       <c r="C170" s="28" t="s">
         <v>170</v>
       </c>
@@ -24624,7 +24667,7 @@
       <c r="A171" s="26">
         <v>25</v>
       </c>
-      <c r="B171" s="74"/>
+      <c r="B171" s="67"/>
       <c r="C171" s="28" t="s">
         <v>171</v>
       </c>
@@ -24644,7 +24687,7 @@
       <c r="A172" s="26">
         <v>26</v>
       </c>
-      <c r="B172" s="74"/>
+      <c r="B172" s="67"/>
       <c r="C172" s="28" t="s">
         <v>40</v>
       </c>
@@ -24664,7 +24707,7 @@
       <c r="A173" s="26">
         <v>27</v>
       </c>
-      <c r="B173" s="75" t="s">
+      <c r="B173" s="66" t="s">
         <v>7</v>
       </c>
       <c r="C173" s="28" t="s">
@@ -24688,7 +24731,7 @@
       <c r="A174" s="26">
         <v>28</v>
       </c>
-      <c r="B174" s="74"/>
+      <c r="B174" s="67"/>
       <c r="C174" s="27" t="s">
         <v>175</v>
       </c>
@@ -24710,7 +24753,7 @@
       <c r="A175" s="26">
         <v>29</v>
       </c>
-      <c r="B175" s="74"/>
+      <c r="B175" s="67"/>
       <c r="C175" s="28" t="s">
         <v>178</v>
       </c>
@@ -24732,7 +24775,7 @@
       <c r="A176" s="26">
         <v>30</v>
       </c>
-      <c r="B176" s="84" t="s">
+      <c r="B176" s="71" t="s">
         <v>8</v>
       </c>
       <c r="C176" s="28" t="s">
@@ -24758,7 +24801,7 @@
       <c r="A177" s="31">
         <v>31</v>
       </c>
-      <c r="B177" s="85"/>
+      <c r="B177" s="72"/>
       <c r="C177" s="32" t="s">
         <v>183</v>
       </c>
@@ -24782,7 +24825,7 @@
       <c r="A178" s="23">
         <v>32</v>
       </c>
-      <c r="B178" s="86" t="s">
+      <c r="B178" s="75" t="s">
         <v>185</v>
       </c>
       <c r="C178" s="33" t="s">
@@ -24806,7 +24849,7 @@
       <c r="A179" s="26">
         <v>33</v>
       </c>
-      <c r="B179" s="87"/>
+      <c r="B179" s="76"/>
       <c r="C179" s="27" t="s">
         <v>189</v>
       </c>
@@ -24828,7 +24871,7 @@
       <c r="A180" s="26">
         <v>34</v>
       </c>
-      <c r="B180" s="88"/>
+      <c r="B180" s="77"/>
       <c r="C180" s="34" t="s">
         <v>192</v>
       </c>
@@ -24850,7 +24893,7 @@
       <c r="A181" s="31">
         <v>35</v>
       </c>
-      <c r="B181" s="88"/>
+      <c r="B181" s="77"/>
       <c r="C181" s="34" t="s">
         <v>193</v>
       </c>
@@ -24872,7 +24915,7 @@
       <c r="A182" s="31">
         <v>36</v>
       </c>
-      <c r="B182" s="88"/>
+      <c r="B182" s="77"/>
       <c r="C182" s="34" t="s">
         <v>196</v>
       </c>
@@ -24892,7 +24935,7 @@
       <c r="A183" s="31">
         <v>37</v>
       </c>
-      <c r="B183" s="88"/>
+      <c r="B183" s="77"/>
       <c r="C183" s="34" t="s">
         <v>248</v>
       </c>
@@ -24914,7 +24957,7 @@
       <c r="A184" s="35">
         <v>38</v>
       </c>
-      <c r="B184" s="83"/>
+      <c r="B184" s="78"/>
       <c r="C184" s="36" t="s">
         <v>252</v>
       </c>
@@ -24965,11 +25008,11 @@
       <c r="B198" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="C198" s="89" t="s">
+      <c r="C198" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="D198" s="89"/>
-      <c r="E198" s="89"/>
+      <c r="D198" s="79"/>
+      <c r="E198" s="79"/>
       <c r="F198" s="37" t="s">
         <v>42</v>
       </c>
@@ -24978,17 +25021,17 @@
       </c>
     </row>
     <row r="199" spans="1:7">
-      <c r="A199" s="72" t="s">
+      <c r="A199" s="80" t="s">
         <v>206</v>
       </c>
-      <c r="B199" s="74" t="s">
+      <c r="B199" s="67" t="s">
         <v>207</v>
       </c>
-      <c r="C199" s="91" t="s">
+      <c r="C199" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="D199" s="92"/>
-      <c r="E199" s="92"/>
+      <c r="D199" s="83"/>
+      <c r="E199" s="83"/>
       <c r="F199" s="28" t="s">
         <v>208</v>
       </c>
@@ -24997,13 +25040,13 @@
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="72"/>
-      <c r="B200" s="90"/>
-      <c r="C200" s="93" t="s">
+      <c r="A200" s="80"/>
+      <c r="B200" s="81"/>
+      <c r="C200" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="D200" s="94"/>
-      <c r="E200" s="94"/>
+      <c r="D200" s="85"/>
+      <c r="E200" s="85"/>
       <c r="F200" s="32" t="s">
         <v>209</v>
       </c>
@@ -25012,15 +25055,15 @@
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="72"/>
-      <c r="B201" s="74" t="s">
+      <c r="A201" s="80"/>
+      <c r="B201" s="67" t="s">
         <v>210</v>
       </c>
-      <c r="C201" s="95" t="s">
+      <c r="C201" s="86" t="s">
         <v>211</v>
       </c>
-      <c r="D201" s="95"/>
-      <c r="E201" s="95"/>
+      <c r="D201" s="86"/>
+      <c r="E201" s="86"/>
       <c r="F201" s="28" t="s">
         <v>208</v>
       </c>
@@ -25029,13 +25072,13 @@
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="72"/>
-      <c r="B202" s="74"/>
-      <c r="C202" s="93" t="s">
+      <c r="A202" s="80"/>
+      <c r="B202" s="67"/>
+      <c r="C202" s="84" t="s">
         <v>211</v>
       </c>
-      <c r="D202" s="93"/>
-      <c r="E202" s="93"/>
+      <c r="D202" s="84"/>
+      <c r="E202" s="84"/>
       <c r="F202" s="28" t="s">
         <v>209</v>
       </c>
@@ -25044,15 +25087,15 @@
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="72"/>
-      <c r="B203" s="90" t="s">
+      <c r="A203" s="80"/>
+      <c r="B203" s="81" t="s">
         <v>212</v>
       </c>
-      <c r="C203" s="96" t="s">
+      <c r="C203" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="D203" s="97"/>
-      <c r="E203" s="98"/>
+      <c r="D203" s="88"/>
+      <c r="E203" s="89"/>
       <c r="F203" s="28" t="s">
         <v>208</v>
       </c>
@@ -25061,13 +25104,13 @@
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="72"/>
-      <c r="B204" s="79"/>
-      <c r="C204" s="96" t="s">
+      <c r="A204" s="80"/>
+      <c r="B204" s="73"/>
+      <c r="C204" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="D204" s="97"/>
-      <c r="E204" s="98"/>
+      <c r="D204" s="88"/>
+      <c r="E204" s="89"/>
       <c r="F204" s="28" t="s">
         <v>209</v>
       </c>
@@ -25076,15 +25119,15 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="72"/>
-      <c r="B205" s="74" t="s">
+      <c r="A205" s="80"/>
+      <c r="B205" s="67" t="s">
         <v>213</v>
       </c>
-      <c r="C205" s="95" t="s">
+      <c r="C205" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="D205" s="95"/>
-      <c r="E205" s="95"/>
+      <c r="D205" s="86"/>
+      <c r="E205" s="86"/>
       <c r="F205" s="28" t="s">
         <v>208</v>
       </c>
@@ -25093,13 +25136,13 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="72"/>
-      <c r="B206" s="74"/>
-      <c r="C206" s="95" t="s">
+      <c r="A206" s="80"/>
+      <c r="B206" s="67"/>
+      <c r="C206" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="D206" s="95"/>
-      <c r="E206" s="95"/>
+      <c r="D206" s="86"/>
+      <c r="E206" s="86"/>
       <c r="F206" s="28" t="s">
         <v>209</v>
       </c>
@@ -25108,17 +25151,17 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="72" t="s">
+      <c r="A207" s="80" t="s">
         <v>215</v>
       </c>
-      <c r="B207" s="74" t="s">
+      <c r="B207" s="67" t="s">
         <v>216</v>
       </c>
-      <c r="C207" s="75" t="s">
+      <c r="C207" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="D207" s="74"/>
-      <c r="E207" s="74"/>
+      <c r="D207" s="67"/>
+      <c r="E207" s="67"/>
       <c r="F207" s="28" t="s">
         <v>208</v>
       </c>
@@ -25127,13 +25170,13 @@
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="72"/>
-      <c r="B208" s="74"/>
-      <c r="C208" s="74" t="s">
+      <c r="A208" s="80"/>
+      <c r="B208" s="67"/>
+      <c r="C208" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="D208" s="74"/>
-      <c r="E208" s="74"/>
+      <c r="D208" s="67"/>
+      <c r="E208" s="67"/>
       <c r="F208" s="28" t="s">
         <v>209</v>
       </c>
@@ -25142,15 +25185,15 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="72"/>
-      <c r="B209" s="74" t="s">
+      <c r="A209" s="80"/>
+      <c r="B209" s="67" t="s">
         <v>218</v>
       </c>
-      <c r="C209" s="74" t="s">
+      <c r="C209" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="D209" s="74"/>
-      <c r="E209" s="74"/>
+      <c r="D209" s="67"/>
+      <c r="E209" s="67"/>
       <c r="F209" s="28" t="s">
         <v>208</v>
       </c>
@@ -25159,13 +25202,13 @@
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="72"/>
-      <c r="B210" s="74"/>
-      <c r="C210" s="74" t="s">
+      <c r="A210" s="80"/>
+      <c r="B210" s="67"/>
+      <c r="C210" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="D210" s="74"/>
-      <c r="E210" s="74"/>
+      <c r="D210" s="67"/>
+      <c r="E210" s="67"/>
       <c r="F210" s="28" t="s">
         <v>209</v>
       </c>
@@ -25174,17 +25217,17 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="72" t="s">
+      <c r="A211" s="80" t="s">
         <v>219</v>
       </c>
-      <c r="B211" s="74" t="s">
+      <c r="B211" s="67" t="s">
         <v>220</v>
       </c>
-      <c r="C211" s="75" t="s">
+      <c r="C211" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="D211" s="74"/>
-      <c r="E211" s="74"/>
+      <c r="D211" s="67"/>
+      <c r="E211" s="67"/>
       <c r="F211" s="28" t="s">
         <v>208</v>
       </c>
@@ -25193,13 +25236,13 @@
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="72"/>
-      <c r="B212" s="74"/>
-      <c r="C212" s="74" t="s">
+      <c r="A212" s="80"/>
+      <c r="B212" s="67"/>
+      <c r="C212" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="D212" s="74"/>
-      <c r="E212" s="74"/>
+      <c r="D212" s="67"/>
+      <c r="E212" s="67"/>
       <c r="F212" s="28" t="s">
         <v>209</v>
       </c>
@@ -25208,15 +25251,15 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="72"/>
-      <c r="B213" s="74" t="s">
+      <c r="A213" s="80"/>
+      <c r="B213" s="67" t="s">
         <v>221</v>
       </c>
-      <c r="C213" s="75" t="s">
+      <c r="C213" s="66" t="s">
         <v>222</v>
       </c>
-      <c r="D213" s="74"/>
-      <c r="E213" s="74"/>
+      <c r="D213" s="67"/>
+      <c r="E213" s="67"/>
       <c r="F213" s="28" t="s">
         <v>208</v>
       </c>
@@ -25225,13 +25268,13 @@
       </c>
     </row>
     <row r="214" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A214" s="73"/>
-      <c r="B214" s="76"/>
-      <c r="C214" s="76" t="s">
+      <c r="A214" s="91"/>
+      <c r="B214" s="92"/>
+      <c r="C214" s="92" t="s">
         <v>223</v>
       </c>
-      <c r="D214" s="76"/>
-      <c r="E214" s="76"/>
+      <c r="D214" s="92"/>
+      <c r="E214" s="92"/>
       <c r="F214" s="36" t="s">
         <v>209</v>
       </c>
@@ -25253,12 +25296,12 @@
       <c r="A219" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="B219" s="77" t="s">
+      <c r="B219" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="C219" s="77"/>
-      <c r="D219" s="77"/>
-      <c r="E219" s="77"/>
+      <c r="C219" s="93"/>
+      <c r="D219" s="93"/>
+      <c r="E219" s="93"/>
       <c r="F219" s="43" t="s">
         <v>227</v>
       </c>
@@ -25270,12 +25313,12 @@
       <c r="A220" s="45" t="s">
         <v>229</v>
       </c>
-      <c r="B220" s="78" t="s">
+      <c r="B220" s="94" t="s">
         <v>230</v>
       </c>
-      <c r="C220" s="79"/>
-      <c r="D220" s="79"/>
-      <c r="E220" s="79"/>
+      <c r="C220" s="73"/>
+      <c r="D220" s="73"/>
+      <c r="E220" s="73"/>
       <c r="F220" s="46" t="s">
         <v>105</v>
       </c>
@@ -25287,12 +25330,12 @@
       <c r="A221" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="B221" s="80" t="s">
+      <c r="B221" s="95" t="s">
         <v>232</v>
       </c>
-      <c r="C221" s="81"/>
-      <c r="D221" s="81"/>
-      <c r="E221" s="82"/>
+      <c r="C221" s="96"/>
+      <c r="D221" s="96"/>
+      <c r="E221" s="97"/>
       <c r="F221" s="15" t="s">
         <v>62</v>
       </c>
@@ -25304,12 +25347,12 @@
       <c r="A222" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B222" s="80" t="s">
+      <c r="B222" s="95" t="s">
         <v>233</v>
       </c>
-      <c r="C222" s="81"/>
-      <c r="D222" s="81"/>
-      <c r="E222" s="82"/>
+      <c r="C222" s="96"/>
+      <c r="D222" s="96"/>
+      <c r="E222" s="97"/>
       <c r="F222" s="18" t="s">
         <v>62</v>
       </c>
@@ -25321,12 +25364,12 @@
       <c r="A223" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="B223" s="83" t="s">
+      <c r="B223" s="78" t="s">
         <v>235</v>
       </c>
-      <c r="C223" s="76"/>
-      <c r="D223" s="76"/>
-      <c r="E223" s="76"/>
+      <c r="C223" s="92"/>
+      <c r="D223" s="92"/>
+      <c r="E223" s="92"/>
       <c r="F223" s="21" t="s">
         <v>62</v>
       </c>
@@ -25371,11 +25414,11 @@
       <c r="C228" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D228" s="71" t="s">
+      <c r="D228" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="E228" s="71"/>
-      <c r="F228" s="71"/>
+      <c r="E228" s="90"/>
+      <c r="F228" s="90"/>
       <c r="G228" s="25"/>
     </row>
     <row r="229" spans="1:7">
@@ -25388,11 +25431,11 @@
       <c r="C229" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D229" s="70" t="s">
+      <c r="D229" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="E229" s="70"/>
-      <c r="F229" s="70"/>
+      <c r="E229" s="102"/>
+      <c r="F229" s="102"/>
       <c r="G229" s="39"/>
     </row>
     <row r="230" spans="1:7">
@@ -25405,11 +25448,11 @@
       <c r="C230" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D230" s="70" t="s">
+      <c r="D230" s="102" t="s">
         <v>239</v>
       </c>
-      <c r="E230" s="70"/>
-      <c r="F230" s="70"/>
+      <c r="E230" s="102"/>
+      <c r="F230" s="102"/>
       <c r="G230" s="39"/>
     </row>
     <row r="231" spans="1:7">
@@ -25422,11 +25465,11 @@
       <c r="C231" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D231" s="70" t="s">
+      <c r="D231" s="102" t="s">
         <v>240</v>
       </c>
-      <c r="E231" s="70"/>
-      <c r="F231" s="70"/>
+      <c r="E231" s="102"/>
+      <c r="F231" s="102"/>
       <c r="G231" s="39"/>
     </row>
     <row r="232" spans="1:7">
@@ -25439,11 +25482,11 @@
       <c r="C232" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D232" s="70" t="s">
+      <c r="D232" s="102" t="s">
         <v>241</v>
       </c>
-      <c r="E232" s="70"/>
-      <c r="F232" s="70"/>
+      <c r="E232" s="102"/>
+      <c r="F232" s="102"/>
       <c r="G232" s="39"/>
     </row>
     <row r="233" spans="1:7">
@@ -25456,11 +25499,11 @@
       <c r="C233" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D233" s="70" t="s">
+      <c r="D233" s="102" t="s">
         <v>242</v>
       </c>
-      <c r="E233" s="70"/>
-      <c r="F233" s="70"/>
+      <c r="E233" s="102"/>
+      <c r="F233" s="102"/>
       <c r="G233" s="39"/>
     </row>
     <row r="234" spans="1:7">
@@ -25473,11 +25516,11 @@
       <c r="C234" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D234" s="66" t="s">
+      <c r="D234" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="E234" s="67"/>
-      <c r="F234" s="68"/>
+      <c r="E234" s="99"/>
+      <c r="F234" s="100"/>
       <c r="G234" s="40"/>
     </row>
     <row r="235" spans="1:7">
@@ -25490,11 +25533,11 @@
       <c r="C235" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D235" s="66" t="s">
+      <c r="D235" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="E235" s="67"/>
-      <c r="F235" s="68"/>
+      <c r="E235" s="99"/>
+      <c r="F235" s="100"/>
       <c r="G235" s="40"/>
     </row>
     <row r="236" spans="1:7">
@@ -25507,11 +25550,11 @@
       <c r="C236" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D236" s="66" t="s">
+      <c r="D236" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="E236" s="67"/>
-      <c r="F236" s="68"/>
+      <c r="E236" s="99"/>
+      <c r="F236" s="100"/>
       <c r="G236" s="40"/>
     </row>
     <row r="237" spans="1:7">
@@ -25592,18 +25635,17 @@
       <c r="C241" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="D241" s="69" t="s">
+      <c r="D241" s="101" t="s">
         <v>255</v>
       </c>
-      <c r="E241" s="69"/>
-      <c r="F241" s="69"/>
+      <c r="E241" s="101"/>
+      <c r="F241" s="101"/>
       <c r="G241" s="41"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ap+vydlQsTivses2kTOZJOfe+E+ofk18ovQVkbwX/cy/2QzQqNYlkd6ZRwhTqYv60tXLJj9O4rjHfeOPlaqbDA==" saltValue="NIz07f4XZ+x9XJy8gC1img==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" scale="115" topLeftCell="A172">
-      <selection activeCell="C180" sqref="C180"/>
+    <customSheetView guid="{FFCBA651-8693-4F31-A4A9-0AA919B68C0C}" scale="115">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -25611,14 +25653,42 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
+    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}" scale="115" topLeftCell="A172">
+      <selection activeCell="C180" sqref="C180"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="B173:B175"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B147:B159"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="B165:B172"/>
+    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D241:F241"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D228:F228"/>
+    <mergeCell ref="A211:A214"/>
+    <mergeCell ref="B211:B212"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="B213:B214"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="B219:E219"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="A207:A210"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="B209:B210"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
     <mergeCell ref="B176:B177"/>
     <mergeCell ref="B178:B184"/>
     <mergeCell ref="C198:E198"/>
@@ -25635,35 +25705,12 @@
     <mergeCell ref="B205:B206"/>
     <mergeCell ref="C205:E205"/>
     <mergeCell ref="C206:E206"/>
-    <mergeCell ref="A207:A210"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="C207:E207"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="B209:B210"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="D228:F228"/>
-    <mergeCell ref="A211:A214"/>
-    <mergeCell ref="B211:B212"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="B213:B214"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="B219:E219"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D241:F241"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="B173:B175"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B147:B159"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="B162:B164"/>
+    <mergeCell ref="B165:B172"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -25686,18 +25733,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}">
+    <customSheetView guid="{FFCBA651-8693-4F31-A4A9-0AA919B68C0C}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="E26" sqref="E26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{0D122794-33D0-4958-A179-FB3706E9A79D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>